<commit_message>
feat:in processing, write type validation
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>user_id: number</t>
+  </si>
+  <si>
+    <t>게시글 삭제</t>
+  </si>
+  <si>
+    <t>delete</t>
   </si>
   <si>
     <t>유저 정보</t>
@@ -308,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -362,6 +368,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -881,28 +890,28 @@
       <c r="Z7" s="16"/>
     </row>
     <row r="8">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="18" t="s">
+        <v>20</v>
+      </c>
       <c r="F8" s="15"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
-      <c r="I8" s="17">
-        <v>200.0</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>39</v>
-      </c>
+      <c r="I8" s="20">
+        <v>204.0</v>
+      </c>
+      <c r="J8" s="15"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
@@ -922,26 +931,26 @@
     </row>
     <row r="9">
       <c r="A9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="16"/>
+      <c r="D9" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="E9" s="16"/>
-      <c r="F9" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="16"/>
       <c r="I9" s="17">
         <v>200.0</v>
       </c>
-      <c r="J9" s="16" t="s">
-        <v>39</v>
+      <c r="J9" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
@@ -962,25 +971,27 @@
     </row>
     <row r="10">
       <c r="A10" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>44</v>
-      </c>
       <c r="C10" s="15" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="15"/>
+      <c r="F10" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
       <c r="I10" s="17">
-        <v>204.0</v>
-      </c>
-      <c r="J10" s="16"/>
+        <v>200.0</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
       <c r="M10" s="16"/>
@@ -999,25 +1010,23 @@
       <c r="Z10" s="16"/>
     </row>
     <row r="11">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="19">
+      <c r="G11" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="15"/>
+      <c r="I11" s="17">
         <v>204.0</v>
       </c>
       <c r="J11" s="16"/>
@@ -1039,2968 +1048,3011 @@
       <c r="Z11" s="16"/>
     </row>
     <row r="12">
-      <c r="I12" s="20"/>
+      <c r="A12" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="19">
+        <v>204.0</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
     </row>
     <row r="13">
-      <c r="I13" s="20"/>
+      <c r="I13" s="21"/>
     </row>
     <row r="14">
-      <c r="I14" s="20"/>
+      <c r="I14" s="21"/>
     </row>
     <row r="15">
-      <c r="I15" s="20"/>
+      <c r="I15" s="21"/>
     </row>
     <row r="16">
-      <c r="I16" s="20"/>
+      <c r="I16" s="21"/>
     </row>
     <row r="17">
-      <c r="I17" s="20"/>
+      <c r="I17" s="21"/>
     </row>
     <row r="18">
-      <c r="I18" s="20"/>
+      <c r="I18" s="21"/>
     </row>
     <row r="19">
-      <c r="I19" s="20"/>
+      <c r="I19" s="21"/>
     </row>
     <row r="20">
-      <c r="I20" s="20"/>
+      <c r="I20" s="21"/>
     </row>
     <row r="21">
-      <c r="I21" s="20"/>
+      <c r="I21" s="21"/>
     </row>
     <row r="22">
-      <c r="I22" s="20"/>
+      <c r="I22" s="21"/>
     </row>
     <row r="23">
-      <c r="I23" s="20"/>
+      <c r="I23" s="21"/>
     </row>
     <row r="24">
-      <c r="I24" s="20"/>
+      <c r="I24" s="21"/>
     </row>
     <row r="25">
-      <c r="I25" s="20"/>
+      <c r="I25" s="21"/>
     </row>
     <row r="26">
-      <c r="I26" s="20"/>
+      <c r="I26" s="21"/>
     </row>
     <row r="27">
-      <c r="I27" s="20"/>
+      <c r="I27" s="21"/>
     </row>
     <row r="28">
-      <c r="I28" s="20"/>
+      <c r="I28" s="21"/>
     </row>
     <row r="29">
-      <c r="I29" s="20"/>
+      <c r="I29" s="21"/>
     </row>
     <row r="30">
-      <c r="I30" s="20"/>
+      <c r="I30" s="21"/>
     </row>
     <row r="31">
-      <c r="I31" s="20"/>
+      <c r="I31" s="21"/>
     </row>
     <row r="32">
-      <c r="I32" s="20"/>
+      <c r="I32" s="21"/>
     </row>
     <row r="33">
-      <c r="I33" s="20"/>
+      <c r="I33" s="21"/>
     </row>
     <row r="34">
-      <c r="I34" s="20"/>
+      <c r="I34" s="21"/>
     </row>
     <row r="35">
-      <c r="I35" s="20"/>
+      <c r="I35" s="21"/>
     </row>
     <row r="36">
-      <c r="I36" s="20"/>
+      <c r="I36" s="21"/>
     </row>
     <row r="37">
-      <c r="I37" s="20"/>
+      <c r="I37" s="21"/>
     </row>
     <row r="38">
-      <c r="I38" s="20"/>
+      <c r="I38" s="21"/>
     </row>
     <row r="39">
-      <c r="I39" s="20"/>
+      <c r="I39" s="21"/>
     </row>
     <row r="40">
-      <c r="I40" s="20"/>
+      <c r="I40" s="21"/>
     </row>
     <row r="41">
-      <c r="I41" s="20"/>
+      <c r="I41" s="21"/>
     </row>
     <row r="42">
-      <c r="I42" s="20"/>
+      <c r="I42" s="21"/>
     </row>
     <row r="43">
-      <c r="I43" s="20"/>
+      <c r="I43" s="21"/>
     </row>
     <row r="44">
-      <c r="I44" s="20"/>
+      <c r="I44" s="21"/>
     </row>
     <row r="45">
-      <c r="I45" s="20"/>
+      <c r="I45" s="21"/>
     </row>
     <row r="46">
-      <c r="I46" s="20"/>
+      <c r="I46" s="21"/>
     </row>
     <row r="47">
-      <c r="I47" s="20"/>
+      <c r="I47" s="21"/>
     </row>
     <row r="48">
-      <c r="I48" s="20"/>
+      <c r="I48" s="21"/>
     </row>
     <row r="49">
-      <c r="I49" s="20"/>
+      <c r="I49" s="21"/>
     </row>
     <row r="50">
-      <c r="I50" s="20"/>
+      <c r="I50" s="21"/>
     </row>
     <row r="51">
-      <c r="I51" s="20"/>
+      <c r="I51" s="21"/>
     </row>
     <row r="52">
-      <c r="I52" s="20"/>
+      <c r="I52" s="21"/>
     </row>
     <row r="53">
-      <c r="I53" s="20"/>
+      <c r="I53" s="21"/>
     </row>
     <row r="54">
-      <c r="I54" s="20"/>
+      <c r="I54" s="21"/>
     </row>
     <row r="55">
-      <c r="I55" s="20"/>
+      <c r="I55" s="21"/>
     </row>
     <row r="56">
-      <c r="I56" s="20"/>
+      <c r="I56" s="21"/>
     </row>
     <row r="57">
-      <c r="I57" s="20"/>
+      <c r="I57" s="21"/>
     </row>
     <row r="58">
-      <c r="I58" s="20"/>
+      <c r="I58" s="21"/>
     </row>
     <row r="59">
-      <c r="I59" s="20"/>
+      <c r="I59" s="21"/>
     </row>
     <row r="60">
-      <c r="I60" s="20"/>
+      <c r="I60" s="21"/>
     </row>
     <row r="61">
-      <c r="I61" s="20"/>
+      <c r="I61" s="21"/>
     </row>
     <row r="62">
-      <c r="I62" s="20"/>
+      <c r="I62" s="21"/>
     </row>
     <row r="63">
-      <c r="I63" s="20"/>
+      <c r="I63" s="21"/>
     </row>
     <row r="64">
-      <c r="I64" s="20"/>
+      <c r="I64" s="21"/>
     </row>
     <row r="65">
-      <c r="I65" s="20"/>
+      <c r="I65" s="21"/>
     </row>
     <row r="66">
-      <c r="I66" s="20"/>
+      <c r="I66" s="21"/>
     </row>
     <row r="67">
-      <c r="I67" s="20"/>
+      <c r="I67" s="21"/>
     </row>
     <row r="68">
-      <c r="I68" s="20"/>
+      <c r="I68" s="21"/>
     </row>
     <row r="69">
-      <c r="I69" s="20"/>
+      <c r="I69" s="21"/>
     </row>
     <row r="70">
-      <c r="I70" s="20"/>
+      <c r="I70" s="21"/>
     </row>
     <row r="71">
-      <c r="I71" s="20"/>
+      <c r="I71" s="21"/>
     </row>
     <row r="72">
-      <c r="I72" s="20"/>
+      <c r="I72" s="21"/>
     </row>
     <row r="73">
-      <c r="I73" s="20"/>
+      <c r="I73" s="21"/>
     </row>
     <row r="74">
-      <c r="I74" s="20"/>
+      <c r="I74" s="21"/>
     </row>
     <row r="75">
-      <c r="I75" s="20"/>
+      <c r="I75" s="21"/>
     </row>
     <row r="76">
-      <c r="I76" s="20"/>
+      <c r="I76" s="21"/>
     </row>
     <row r="77">
-      <c r="I77" s="20"/>
+      <c r="I77" s="21"/>
     </row>
     <row r="78">
-      <c r="I78" s="20"/>
+      <c r="I78" s="21"/>
     </row>
     <row r="79">
-      <c r="I79" s="20"/>
+      <c r="I79" s="21"/>
     </row>
     <row r="80">
-      <c r="I80" s="20"/>
+      <c r="I80" s="21"/>
     </row>
     <row r="81">
-      <c r="I81" s="20"/>
+      <c r="I81" s="21"/>
     </row>
     <row r="82">
-      <c r="I82" s="20"/>
+      <c r="I82" s="21"/>
     </row>
     <row r="83">
-      <c r="I83" s="20"/>
+      <c r="I83" s="21"/>
     </row>
     <row r="84">
-      <c r="I84" s="20"/>
+      <c r="I84" s="21"/>
     </row>
     <row r="85">
-      <c r="I85" s="20"/>
+      <c r="I85" s="21"/>
     </row>
     <row r="86">
-      <c r="I86" s="20"/>
+      <c r="I86" s="21"/>
     </row>
     <row r="87">
-      <c r="I87" s="20"/>
+      <c r="I87" s="21"/>
     </row>
     <row r="88">
-      <c r="I88" s="20"/>
+      <c r="I88" s="21"/>
     </row>
     <row r="89">
-      <c r="I89" s="20"/>
+      <c r="I89" s="21"/>
     </row>
     <row r="90">
-      <c r="I90" s="20"/>
+      <c r="I90" s="21"/>
     </row>
     <row r="91">
-      <c r="I91" s="20"/>
+      <c r="I91" s="21"/>
     </row>
     <row r="92">
-      <c r="I92" s="20"/>
+      <c r="I92" s="21"/>
     </row>
     <row r="93">
-      <c r="I93" s="20"/>
+      <c r="I93" s="21"/>
     </row>
     <row r="94">
-      <c r="I94" s="20"/>
+      <c r="I94" s="21"/>
     </row>
     <row r="95">
-      <c r="I95" s="20"/>
+      <c r="I95" s="21"/>
     </row>
     <row r="96">
-      <c r="I96" s="20"/>
+      <c r="I96" s="21"/>
     </row>
     <row r="97">
-      <c r="I97" s="20"/>
+      <c r="I97" s="21"/>
     </row>
     <row r="98">
-      <c r="I98" s="20"/>
+      <c r="I98" s="21"/>
     </row>
     <row r="99">
-      <c r="I99" s="20"/>
+      <c r="I99" s="21"/>
     </row>
     <row r="100">
-      <c r="I100" s="20"/>
+      <c r="I100" s="21"/>
     </row>
     <row r="101">
-      <c r="I101" s="20"/>
+      <c r="I101" s="21"/>
     </row>
     <row r="102">
-      <c r="I102" s="20"/>
+      <c r="I102" s="21"/>
     </row>
     <row r="103">
-      <c r="I103" s="20"/>
+      <c r="I103" s="21"/>
     </row>
     <row r="104">
-      <c r="I104" s="20"/>
+      <c r="I104" s="21"/>
     </row>
     <row r="105">
-      <c r="I105" s="20"/>
+      <c r="I105" s="21"/>
     </row>
     <row r="106">
-      <c r="I106" s="20"/>
+      <c r="I106" s="21"/>
     </row>
     <row r="107">
-      <c r="I107" s="20"/>
+      <c r="I107" s="21"/>
     </row>
     <row r="108">
-      <c r="I108" s="20"/>
+      <c r="I108" s="21"/>
     </row>
     <row r="109">
-      <c r="I109" s="20"/>
+      <c r="I109" s="21"/>
     </row>
     <row r="110">
-      <c r="I110" s="20"/>
+      <c r="I110" s="21"/>
     </row>
     <row r="111">
-      <c r="I111" s="20"/>
+      <c r="I111" s="21"/>
     </row>
     <row r="112">
-      <c r="I112" s="20"/>
+      <c r="I112" s="21"/>
     </row>
     <row r="113">
-      <c r="I113" s="20"/>
+      <c r="I113" s="21"/>
     </row>
     <row r="114">
-      <c r="I114" s="20"/>
+      <c r="I114" s="21"/>
     </row>
     <row r="115">
-      <c r="I115" s="20"/>
+      <c r="I115" s="21"/>
     </row>
     <row r="116">
-      <c r="I116" s="20"/>
+      <c r="I116" s="21"/>
     </row>
     <row r="117">
-      <c r="I117" s="20"/>
+      <c r="I117" s="21"/>
     </row>
     <row r="118">
-      <c r="I118" s="20"/>
+      <c r="I118" s="21"/>
     </row>
     <row r="119">
-      <c r="I119" s="20"/>
+      <c r="I119" s="21"/>
     </row>
     <row r="120">
-      <c r="I120" s="20"/>
+      <c r="I120" s="21"/>
     </row>
     <row r="121">
-      <c r="I121" s="20"/>
+      <c r="I121" s="21"/>
     </row>
     <row r="122">
-      <c r="I122" s="20"/>
+      <c r="I122" s="21"/>
     </row>
     <row r="123">
-      <c r="I123" s="20"/>
+      <c r="I123" s="21"/>
     </row>
     <row r="124">
-      <c r="I124" s="20"/>
+      <c r="I124" s="21"/>
     </row>
     <row r="125">
-      <c r="I125" s="20"/>
+      <c r="I125" s="21"/>
     </row>
     <row r="126">
-      <c r="I126" s="20"/>
+      <c r="I126" s="21"/>
     </row>
     <row r="127">
-      <c r="I127" s="20"/>
+      <c r="I127" s="21"/>
     </row>
     <row r="128">
-      <c r="I128" s="20"/>
+      <c r="I128" s="21"/>
     </row>
     <row r="129">
-      <c r="I129" s="20"/>
+      <c r="I129" s="21"/>
     </row>
     <row r="130">
-      <c r="I130" s="20"/>
+      <c r="I130" s="21"/>
     </row>
     <row r="131">
-      <c r="I131" s="20"/>
+      <c r="I131" s="21"/>
     </row>
     <row r="132">
-      <c r="I132" s="20"/>
+      <c r="I132" s="21"/>
     </row>
     <row r="133">
-      <c r="I133" s="20"/>
+      <c r="I133" s="21"/>
     </row>
     <row r="134">
-      <c r="I134" s="20"/>
+      <c r="I134" s="21"/>
     </row>
     <row r="135">
-      <c r="I135" s="20"/>
+      <c r="I135" s="21"/>
     </row>
     <row r="136">
-      <c r="I136" s="20"/>
+      <c r="I136" s="21"/>
     </row>
     <row r="137">
-      <c r="I137" s="20"/>
+      <c r="I137" s="21"/>
     </row>
     <row r="138">
-      <c r="I138" s="20"/>
+      <c r="I138" s="21"/>
     </row>
     <row r="139">
-      <c r="I139" s="20"/>
+      <c r="I139" s="21"/>
     </row>
     <row r="140">
-      <c r="I140" s="20"/>
+      <c r="I140" s="21"/>
     </row>
     <row r="141">
-      <c r="I141" s="20"/>
+      <c r="I141" s="21"/>
     </row>
     <row r="142">
-      <c r="I142" s="20"/>
+      <c r="I142" s="21"/>
     </row>
     <row r="143">
-      <c r="I143" s="20"/>
+      <c r="I143" s="21"/>
     </row>
     <row r="144">
-      <c r="I144" s="20"/>
+      <c r="I144" s="21"/>
     </row>
     <row r="145">
-      <c r="I145" s="20"/>
+      <c r="I145" s="21"/>
     </row>
     <row r="146">
-      <c r="I146" s="20"/>
+      <c r="I146" s="21"/>
     </row>
     <row r="147">
-      <c r="I147" s="20"/>
+      <c r="I147" s="21"/>
     </row>
     <row r="148">
-      <c r="I148" s="20"/>
+      <c r="I148" s="21"/>
     </row>
     <row r="149">
-      <c r="I149" s="20"/>
+      <c r="I149" s="21"/>
     </row>
     <row r="150">
-      <c r="I150" s="20"/>
+      <c r="I150" s="21"/>
     </row>
     <row r="151">
-      <c r="I151" s="20"/>
+      <c r="I151" s="21"/>
     </row>
     <row r="152">
-      <c r="I152" s="20"/>
+      <c r="I152" s="21"/>
     </row>
     <row r="153">
-      <c r="I153" s="20"/>
+      <c r="I153" s="21"/>
     </row>
     <row r="154">
-      <c r="I154" s="20"/>
+      <c r="I154" s="21"/>
     </row>
     <row r="155">
-      <c r="I155" s="20"/>
+      <c r="I155" s="21"/>
     </row>
     <row r="156">
-      <c r="I156" s="20"/>
+      <c r="I156" s="21"/>
     </row>
     <row r="157">
-      <c r="I157" s="20"/>
+      <c r="I157" s="21"/>
     </row>
     <row r="158">
-      <c r="I158" s="20"/>
+      <c r="I158" s="21"/>
     </row>
     <row r="159">
-      <c r="I159" s="20"/>
+      <c r="I159" s="21"/>
     </row>
     <row r="160">
-      <c r="I160" s="20"/>
+      <c r="I160" s="21"/>
     </row>
     <row r="161">
-      <c r="I161" s="20"/>
+      <c r="I161" s="21"/>
     </row>
     <row r="162">
-      <c r="I162" s="20"/>
+      <c r="I162" s="21"/>
     </row>
     <row r="163">
-      <c r="I163" s="20"/>
+      <c r="I163" s="21"/>
     </row>
     <row r="164">
-      <c r="I164" s="20"/>
+      <c r="I164" s="21"/>
     </row>
     <row r="165">
-      <c r="I165" s="20"/>
+      <c r="I165" s="21"/>
     </row>
     <row r="166">
-      <c r="I166" s="20"/>
+      <c r="I166" s="21"/>
     </row>
     <row r="167">
-      <c r="I167" s="20"/>
+      <c r="I167" s="21"/>
     </row>
     <row r="168">
-      <c r="I168" s="20"/>
+      <c r="I168" s="21"/>
     </row>
     <row r="169">
-      <c r="I169" s="20"/>
+      <c r="I169" s="21"/>
     </row>
     <row r="170">
-      <c r="I170" s="20"/>
+      <c r="I170" s="21"/>
     </row>
     <row r="171">
-      <c r="I171" s="20"/>
+      <c r="I171" s="21"/>
     </row>
     <row r="172">
-      <c r="I172" s="20"/>
+      <c r="I172" s="21"/>
     </row>
     <row r="173">
-      <c r="I173" s="20"/>
+      <c r="I173" s="21"/>
     </row>
     <row r="174">
-      <c r="I174" s="20"/>
+      <c r="I174" s="21"/>
     </row>
     <row r="175">
-      <c r="I175" s="20"/>
+      <c r="I175" s="21"/>
     </row>
     <row r="176">
-      <c r="I176" s="20"/>
+      <c r="I176" s="21"/>
     </row>
     <row r="177">
-      <c r="I177" s="20"/>
+      <c r="I177" s="21"/>
     </row>
     <row r="178">
-      <c r="I178" s="20"/>
+      <c r="I178" s="21"/>
     </row>
     <row r="179">
-      <c r="I179" s="20"/>
+      <c r="I179" s="21"/>
     </row>
     <row r="180">
-      <c r="I180" s="20"/>
+      <c r="I180" s="21"/>
     </row>
     <row r="181">
-      <c r="I181" s="20"/>
+      <c r="I181" s="21"/>
     </row>
     <row r="182">
-      <c r="I182" s="20"/>
+      <c r="I182" s="21"/>
     </row>
     <row r="183">
-      <c r="I183" s="20"/>
+      <c r="I183" s="21"/>
     </row>
     <row r="184">
-      <c r="I184" s="20"/>
+      <c r="I184" s="21"/>
     </row>
     <row r="185">
-      <c r="I185" s="20"/>
+      <c r="I185" s="21"/>
     </row>
     <row r="186">
-      <c r="I186" s="20"/>
+      <c r="I186" s="21"/>
     </row>
     <row r="187">
-      <c r="I187" s="20"/>
+      <c r="I187" s="21"/>
     </row>
     <row r="188">
-      <c r="I188" s="20"/>
+      <c r="I188" s="21"/>
     </row>
     <row r="189">
-      <c r="I189" s="20"/>
+      <c r="I189" s="21"/>
     </row>
     <row r="190">
-      <c r="I190" s="20"/>
+      <c r="I190" s="21"/>
     </row>
     <row r="191">
-      <c r="I191" s="20"/>
+      <c r="I191" s="21"/>
     </row>
     <row r="192">
-      <c r="I192" s="20"/>
+      <c r="I192" s="21"/>
     </row>
     <row r="193">
-      <c r="I193" s="20"/>
+      <c r="I193" s="21"/>
     </row>
     <row r="194">
-      <c r="I194" s="20"/>
+      <c r="I194" s="21"/>
     </row>
     <row r="195">
-      <c r="I195" s="20"/>
+      <c r="I195" s="21"/>
     </row>
     <row r="196">
-      <c r="I196" s="20"/>
+      <c r="I196" s="21"/>
     </row>
     <row r="197">
-      <c r="I197" s="20"/>
+      <c r="I197" s="21"/>
     </row>
     <row r="198">
-      <c r="I198" s="20"/>
+      <c r="I198" s="21"/>
     </row>
     <row r="199">
-      <c r="I199" s="20"/>
+      <c r="I199" s="21"/>
     </row>
     <row r="200">
-      <c r="I200" s="20"/>
+      <c r="I200" s="21"/>
     </row>
     <row r="201">
-      <c r="I201" s="20"/>
+      <c r="I201" s="21"/>
     </row>
     <row r="202">
-      <c r="I202" s="20"/>
+      <c r="I202" s="21"/>
     </row>
     <row r="203">
-      <c r="I203" s="20"/>
+      <c r="I203" s="21"/>
     </row>
     <row r="204">
-      <c r="I204" s="20"/>
+      <c r="I204" s="21"/>
     </row>
     <row r="205">
-      <c r="I205" s="20"/>
+      <c r="I205" s="21"/>
     </row>
     <row r="206">
-      <c r="I206" s="20"/>
+      <c r="I206" s="21"/>
     </row>
     <row r="207">
-      <c r="I207" s="20"/>
+      <c r="I207" s="21"/>
     </row>
     <row r="208">
-      <c r="I208" s="20"/>
+      <c r="I208" s="21"/>
     </row>
     <row r="209">
-      <c r="I209" s="20"/>
+      <c r="I209" s="21"/>
     </row>
     <row r="210">
-      <c r="I210" s="20"/>
+      <c r="I210" s="21"/>
     </row>
     <row r="211">
-      <c r="I211" s="20"/>
+      <c r="I211" s="21"/>
     </row>
     <row r="212">
-      <c r="I212" s="20"/>
+      <c r="I212" s="21"/>
     </row>
     <row r="213">
-      <c r="I213" s="20"/>
+      <c r="I213" s="21"/>
     </row>
     <row r="214">
-      <c r="I214" s="20"/>
+      <c r="I214" s="21"/>
     </row>
     <row r="215">
-      <c r="I215" s="20"/>
+      <c r="I215" s="21"/>
     </row>
     <row r="216">
-      <c r="I216" s="20"/>
+      <c r="I216" s="21"/>
     </row>
     <row r="217">
-      <c r="I217" s="20"/>
+      <c r="I217" s="21"/>
     </row>
     <row r="218">
-      <c r="I218" s="20"/>
+      <c r="I218" s="21"/>
     </row>
     <row r="219">
-      <c r="I219" s="20"/>
+      <c r="I219" s="21"/>
     </row>
     <row r="220">
-      <c r="I220" s="20"/>
+      <c r="I220" s="21"/>
     </row>
     <row r="221">
-      <c r="I221" s="20"/>
+      <c r="I221" s="21"/>
     </row>
     <row r="222">
-      <c r="I222" s="20"/>
+      <c r="I222" s="21"/>
     </row>
     <row r="223">
-      <c r="I223" s="20"/>
+      <c r="I223" s="21"/>
     </row>
     <row r="224">
-      <c r="I224" s="20"/>
+      <c r="I224" s="21"/>
     </row>
     <row r="225">
-      <c r="I225" s="20"/>
+      <c r="I225" s="21"/>
     </row>
     <row r="226">
-      <c r="I226" s="20"/>
+      <c r="I226" s="21"/>
     </row>
     <row r="227">
-      <c r="I227" s="20"/>
+      <c r="I227" s="21"/>
     </row>
     <row r="228">
-      <c r="I228" s="20"/>
+      <c r="I228" s="21"/>
     </row>
     <row r="229">
-      <c r="I229" s="20"/>
+      <c r="I229" s="21"/>
     </row>
     <row r="230">
-      <c r="I230" s="20"/>
+      <c r="I230" s="21"/>
     </row>
     <row r="231">
-      <c r="I231" s="20"/>
+      <c r="I231" s="21"/>
     </row>
     <row r="232">
-      <c r="I232" s="20"/>
+      <c r="I232" s="21"/>
     </row>
     <row r="233">
-      <c r="I233" s="20"/>
+      <c r="I233" s="21"/>
     </row>
     <row r="234">
-      <c r="I234" s="20"/>
+      <c r="I234" s="21"/>
     </row>
     <row r="235">
-      <c r="I235" s="20"/>
+      <c r="I235" s="21"/>
     </row>
     <row r="236">
-      <c r="I236" s="20"/>
+      <c r="I236" s="21"/>
     </row>
     <row r="237">
-      <c r="I237" s="20"/>
+      <c r="I237" s="21"/>
     </row>
     <row r="238">
-      <c r="I238" s="20"/>
+      <c r="I238" s="21"/>
     </row>
     <row r="239">
-      <c r="I239" s="20"/>
+      <c r="I239" s="21"/>
     </row>
     <row r="240">
-      <c r="I240" s="20"/>
+      <c r="I240" s="21"/>
     </row>
     <row r="241">
-      <c r="I241" s="20"/>
+      <c r="I241" s="21"/>
     </row>
     <row r="242">
-      <c r="I242" s="20"/>
+      <c r="I242" s="21"/>
     </row>
     <row r="243">
-      <c r="I243" s="20"/>
+      <c r="I243" s="21"/>
     </row>
     <row r="244">
-      <c r="I244" s="20"/>
+      <c r="I244" s="21"/>
     </row>
     <row r="245">
-      <c r="I245" s="20"/>
+      <c r="I245" s="21"/>
     </row>
     <row r="246">
-      <c r="I246" s="20"/>
+      <c r="I246" s="21"/>
     </row>
     <row r="247">
-      <c r="I247" s="20"/>
+      <c r="I247" s="21"/>
     </row>
     <row r="248">
-      <c r="I248" s="20"/>
+      <c r="I248" s="21"/>
     </row>
     <row r="249">
-      <c r="I249" s="20"/>
+      <c r="I249" s="21"/>
     </row>
     <row r="250">
-      <c r="I250" s="20"/>
+      <c r="I250" s="21"/>
     </row>
     <row r="251">
-      <c r="I251" s="20"/>
+      <c r="I251" s="21"/>
     </row>
     <row r="252">
-      <c r="I252" s="20"/>
+      <c r="I252" s="21"/>
     </row>
     <row r="253">
-      <c r="I253" s="20"/>
+      <c r="I253" s="21"/>
     </row>
     <row r="254">
-      <c r="I254" s="20"/>
+      <c r="I254" s="21"/>
     </row>
     <row r="255">
-      <c r="I255" s="20"/>
+      <c r="I255" s="21"/>
     </row>
     <row r="256">
-      <c r="I256" s="20"/>
+      <c r="I256" s="21"/>
     </row>
     <row r="257">
-      <c r="I257" s="20"/>
+      <c r="I257" s="21"/>
     </row>
     <row r="258">
-      <c r="I258" s="20"/>
+      <c r="I258" s="21"/>
     </row>
     <row r="259">
-      <c r="I259" s="20"/>
+      <c r="I259" s="21"/>
     </row>
     <row r="260">
-      <c r="I260" s="20"/>
+      <c r="I260" s="21"/>
     </row>
     <row r="261">
-      <c r="I261" s="20"/>
+      <c r="I261" s="21"/>
     </row>
     <row r="262">
-      <c r="I262" s="20"/>
+      <c r="I262" s="21"/>
     </row>
     <row r="263">
-      <c r="I263" s="20"/>
+      <c r="I263" s="21"/>
     </row>
     <row r="264">
-      <c r="I264" s="20"/>
+      <c r="I264" s="21"/>
     </row>
     <row r="265">
-      <c r="I265" s="20"/>
+      <c r="I265" s="21"/>
     </row>
     <row r="266">
-      <c r="I266" s="20"/>
+      <c r="I266" s="21"/>
     </row>
     <row r="267">
-      <c r="I267" s="20"/>
+      <c r="I267" s="21"/>
     </row>
     <row r="268">
-      <c r="I268" s="20"/>
+      <c r="I268" s="21"/>
     </row>
     <row r="269">
-      <c r="I269" s="20"/>
+      <c r="I269" s="21"/>
     </row>
     <row r="270">
-      <c r="I270" s="20"/>
+      <c r="I270" s="21"/>
     </row>
     <row r="271">
-      <c r="I271" s="20"/>
+      <c r="I271" s="21"/>
     </row>
     <row r="272">
-      <c r="I272" s="20"/>
+      <c r="I272" s="21"/>
     </row>
     <row r="273">
-      <c r="I273" s="20"/>
+      <c r="I273" s="21"/>
     </row>
     <row r="274">
-      <c r="I274" s="20"/>
+      <c r="I274" s="21"/>
     </row>
     <row r="275">
-      <c r="I275" s="20"/>
+      <c r="I275" s="21"/>
     </row>
     <row r="276">
-      <c r="I276" s="20"/>
+      <c r="I276" s="21"/>
     </row>
     <row r="277">
-      <c r="I277" s="20"/>
+      <c r="I277" s="21"/>
     </row>
     <row r="278">
-      <c r="I278" s="20"/>
+      <c r="I278" s="21"/>
     </row>
     <row r="279">
-      <c r="I279" s="20"/>
+      <c r="I279" s="21"/>
     </row>
     <row r="280">
-      <c r="I280" s="20"/>
+      <c r="I280" s="21"/>
     </row>
     <row r="281">
-      <c r="I281" s="20"/>
+      <c r="I281" s="21"/>
     </row>
     <row r="282">
-      <c r="I282" s="20"/>
+      <c r="I282" s="21"/>
     </row>
     <row r="283">
-      <c r="I283" s="20"/>
+      <c r="I283" s="21"/>
     </row>
     <row r="284">
-      <c r="I284" s="20"/>
+      <c r="I284" s="21"/>
     </row>
     <row r="285">
-      <c r="I285" s="20"/>
+      <c r="I285" s="21"/>
     </row>
     <row r="286">
-      <c r="I286" s="20"/>
+      <c r="I286" s="21"/>
     </row>
     <row r="287">
-      <c r="I287" s="20"/>
+      <c r="I287" s="21"/>
     </row>
     <row r="288">
-      <c r="I288" s="20"/>
+      <c r="I288" s="21"/>
     </row>
     <row r="289">
-      <c r="I289" s="20"/>
+      <c r="I289" s="21"/>
     </row>
     <row r="290">
-      <c r="I290" s="20"/>
+      <c r="I290" s="21"/>
     </row>
     <row r="291">
-      <c r="I291" s="20"/>
+      <c r="I291" s="21"/>
     </row>
     <row r="292">
-      <c r="I292" s="20"/>
+      <c r="I292" s="21"/>
     </row>
     <row r="293">
-      <c r="I293" s="20"/>
+      <c r="I293" s="21"/>
     </row>
     <row r="294">
-      <c r="I294" s="20"/>
+      <c r="I294" s="21"/>
     </row>
     <row r="295">
-      <c r="I295" s="20"/>
+      <c r="I295" s="21"/>
     </row>
     <row r="296">
-      <c r="I296" s="20"/>
+      <c r="I296" s="21"/>
     </row>
     <row r="297">
-      <c r="I297" s="20"/>
+      <c r="I297" s="21"/>
     </row>
     <row r="298">
-      <c r="I298" s="20"/>
+      <c r="I298" s="21"/>
     </row>
     <row r="299">
-      <c r="I299" s="20"/>
+      <c r="I299" s="21"/>
     </row>
     <row r="300">
-      <c r="I300" s="20"/>
+      <c r="I300" s="21"/>
     </row>
     <row r="301">
-      <c r="I301" s="20"/>
+      <c r="I301" s="21"/>
     </row>
     <row r="302">
-      <c r="I302" s="20"/>
+      <c r="I302" s="21"/>
     </row>
     <row r="303">
-      <c r="I303" s="20"/>
+      <c r="I303" s="21"/>
     </row>
     <row r="304">
-      <c r="I304" s="20"/>
+      <c r="I304" s="21"/>
     </row>
     <row r="305">
-      <c r="I305" s="20"/>
+      <c r="I305" s="21"/>
     </row>
     <row r="306">
-      <c r="I306" s="20"/>
+      <c r="I306" s="21"/>
     </row>
     <row r="307">
-      <c r="I307" s="20"/>
+      <c r="I307" s="21"/>
     </row>
     <row r="308">
-      <c r="I308" s="20"/>
+      <c r="I308" s="21"/>
     </row>
     <row r="309">
-      <c r="I309" s="20"/>
+      <c r="I309" s="21"/>
     </row>
     <row r="310">
-      <c r="I310" s="20"/>
+      <c r="I310" s="21"/>
     </row>
     <row r="311">
-      <c r="I311" s="20"/>
+      <c r="I311" s="21"/>
     </row>
     <row r="312">
-      <c r="I312" s="20"/>
+      <c r="I312" s="21"/>
     </row>
     <row r="313">
-      <c r="I313" s="20"/>
+      <c r="I313" s="21"/>
     </row>
     <row r="314">
-      <c r="I314" s="20"/>
+      <c r="I314" s="21"/>
     </row>
     <row r="315">
-      <c r="I315" s="20"/>
+      <c r="I315" s="21"/>
     </row>
     <row r="316">
-      <c r="I316" s="20"/>
+      <c r="I316" s="21"/>
     </row>
     <row r="317">
-      <c r="I317" s="20"/>
+      <c r="I317" s="21"/>
     </row>
     <row r="318">
-      <c r="I318" s="20"/>
+      <c r="I318" s="21"/>
     </row>
     <row r="319">
-      <c r="I319" s="20"/>
+      <c r="I319" s="21"/>
     </row>
     <row r="320">
-      <c r="I320" s="20"/>
+      <c r="I320" s="21"/>
     </row>
     <row r="321">
-      <c r="I321" s="20"/>
+      <c r="I321" s="21"/>
     </row>
     <row r="322">
-      <c r="I322" s="20"/>
+      <c r="I322" s="21"/>
     </row>
     <row r="323">
-      <c r="I323" s="20"/>
+      <c r="I323" s="21"/>
     </row>
     <row r="324">
-      <c r="I324" s="20"/>
+      <c r="I324" s="21"/>
     </row>
     <row r="325">
-      <c r="I325" s="20"/>
+      <c r="I325" s="21"/>
     </row>
     <row r="326">
-      <c r="I326" s="20"/>
+      <c r="I326" s="21"/>
     </row>
     <row r="327">
-      <c r="I327" s="20"/>
+      <c r="I327" s="21"/>
     </row>
     <row r="328">
-      <c r="I328" s="20"/>
+      <c r="I328" s="21"/>
     </row>
     <row r="329">
-      <c r="I329" s="20"/>
+      <c r="I329" s="21"/>
     </row>
     <row r="330">
-      <c r="I330" s="20"/>
+      <c r="I330" s="21"/>
     </row>
     <row r="331">
-      <c r="I331" s="20"/>
+      <c r="I331" s="21"/>
     </row>
     <row r="332">
-      <c r="I332" s="20"/>
+      <c r="I332" s="21"/>
     </row>
     <row r="333">
-      <c r="I333" s="20"/>
+      <c r="I333" s="21"/>
     </row>
     <row r="334">
-      <c r="I334" s="20"/>
+      <c r="I334" s="21"/>
     </row>
     <row r="335">
-      <c r="I335" s="20"/>
+      <c r="I335" s="21"/>
     </row>
     <row r="336">
-      <c r="I336" s="20"/>
+      <c r="I336" s="21"/>
     </row>
     <row r="337">
-      <c r="I337" s="20"/>
+      <c r="I337" s="21"/>
     </row>
     <row r="338">
-      <c r="I338" s="20"/>
+      <c r="I338" s="21"/>
     </row>
     <row r="339">
-      <c r="I339" s="20"/>
+      <c r="I339" s="21"/>
     </row>
     <row r="340">
-      <c r="I340" s="20"/>
+      <c r="I340" s="21"/>
     </row>
     <row r="341">
-      <c r="I341" s="20"/>
+      <c r="I341" s="21"/>
     </row>
     <row r="342">
-      <c r="I342" s="20"/>
+      <c r="I342" s="21"/>
     </row>
     <row r="343">
-      <c r="I343" s="20"/>
+      <c r="I343" s="21"/>
     </row>
     <row r="344">
-      <c r="I344" s="20"/>
+      <c r="I344" s="21"/>
     </row>
     <row r="345">
-      <c r="I345" s="20"/>
+      <c r="I345" s="21"/>
     </row>
     <row r="346">
-      <c r="I346" s="20"/>
+      <c r="I346" s="21"/>
     </row>
     <row r="347">
-      <c r="I347" s="20"/>
+      <c r="I347" s="21"/>
     </row>
     <row r="348">
-      <c r="I348" s="20"/>
+      <c r="I348" s="21"/>
     </row>
     <row r="349">
-      <c r="I349" s="20"/>
+      <c r="I349" s="21"/>
     </row>
     <row r="350">
-      <c r="I350" s="20"/>
+      <c r="I350" s="21"/>
     </row>
     <row r="351">
-      <c r="I351" s="20"/>
+      <c r="I351" s="21"/>
     </row>
     <row r="352">
-      <c r="I352" s="20"/>
+      <c r="I352" s="21"/>
     </row>
     <row r="353">
-      <c r="I353" s="20"/>
+      <c r="I353" s="21"/>
     </row>
     <row r="354">
-      <c r="I354" s="20"/>
+      <c r="I354" s="21"/>
     </row>
     <row r="355">
-      <c r="I355" s="20"/>
+      <c r="I355" s="21"/>
     </row>
     <row r="356">
-      <c r="I356" s="20"/>
+      <c r="I356" s="21"/>
     </row>
     <row r="357">
-      <c r="I357" s="20"/>
+      <c r="I357" s="21"/>
     </row>
     <row r="358">
-      <c r="I358" s="20"/>
+      <c r="I358" s="21"/>
     </row>
     <row r="359">
-      <c r="I359" s="20"/>
+      <c r="I359" s="21"/>
     </row>
     <row r="360">
-      <c r="I360" s="20"/>
+      <c r="I360" s="21"/>
     </row>
     <row r="361">
-      <c r="I361" s="20"/>
+      <c r="I361" s="21"/>
     </row>
     <row r="362">
-      <c r="I362" s="20"/>
+      <c r="I362" s="21"/>
     </row>
     <row r="363">
-      <c r="I363" s="20"/>
+      <c r="I363" s="21"/>
     </row>
     <row r="364">
-      <c r="I364" s="20"/>
+      <c r="I364" s="21"/>
     </row>
     <row r="365">
-      <c r="I365" s="20"/>
+      <c r="I365" s="21"/>
     </row>
     <row r="366">
-      <c r="I366" s="20"/>
+      <c r="I366" s="21"/>
     </row>
     <row r="367">
-      <c r="I367" s="20"/>
+      <c r="I367" s="21"/>
     </row>
     <row r="368">
-      <c r="I368" s="20"/>
+      <c r="I368" s="21"/>
     </row>
     <row r="369">
-      <c r="I369" s="20"/>
+      <c r="I369" s="21"/>
     </row>
     <row r="370">
-      <c r="I370" s="20"/>
+      <c r="I370" s="21"/>
     </row>
     <row r="371">
-      <c r="I371" s="20"/>
+      <c r="I371" s="21"/>
     </row>
     <row r="372">
-      <c r="I372" s="20"/>
+      <c r="I372" s="21"/>
     </row>
     <row r="373">
-      <c r="I373" s="20"/>
+      <c r="I373" s="21"/>
     </row>
     <row r="374">
-      <c r="I374" s="20"/>
+      <c r="I374" s="21"/>
     </row>
     <row r="375">
-      <c r="I375" s="20"/>
+      <c r="I375" s="21"/>
     </row>
     <row r="376">
-      <c r="I376" s="20"/>
+      <c r="I376" s="21"/>
     </row>
     <row r="377">
-      <c r="I377" s="20"/>
+      <c r="I377" s="21"/>
     </row>
     <row r="378">
-      <c r="I378" s="20"/>
+      <c r="I378" s="21"/>
     </row>
     <row r="379">
-      <c r="I379" s="20"/>
+      <c r="I379" s="21"/>
     </row>
     <row r="380">
-      <c r="I380" s="20"/>
+      <c r="I380" s="21"/>
     </row>
     <row r="381">
-      <c r="I381" s="20"/>
+      <c r="I381" s="21"/>
     </row>
     <row r="382">
-      <c r="I382" s="20"/>
+      <c r="I382" s="21"/>
     </row>
     <row r="383">
-      <c r="I383" s="20"/>
+      <c r="I383" s="21"/>
     </row>
     <row r="384">
-      <c r="I384" s="20"/>
+      <c r="I384" s="21"/>
     </row>
     <row r="385">
-      <c r="I385" s="20"/>
+      <c r="I385" s="21"/>
     </row>
     <row r="386">
-      <c r="I386" s="20"/>
+      <c r="I386" s="21"/>
     </row>
     <row r="387">
-      <c r="I387" s="20"/>
+      <c r="I387" s="21"/>
     </row>
     <row r="388">
-      <c r="I388" s="20"/>
+      <c r="I388" s="21"/>
     </row>
     <row r="389">
-      <c r="I389" s="20"/>
+      <c r="I389" s="21"/>
     </row>
     <row r="390">
-      <c r="I390" s="20"/>
+      <c r="I390" s="21"/>
     </row>
     <row r="391">
-      <c r="I391" s="20"/>
+      <c r="I391" s="21"/>
     </row>
     <row r="392">
-      <c r="I392" s="20"/>
+      <c r="I392" s="21"/>
     </row>
     <row r="393">
-      <c r="I393" s="20"/>
+      <c r="I393" s="21"/>
     </row>
     <row r="394">
-      <c r="I394" s="20"/>
+      <c r="I394" s="21"/>
     </row>
     <row r="395">
-      <c r="I395" s="20"/>
+      <c r="I395" s="21"/>
     </row>
     <row r="396">
-      <c r="I396" s="20"/>
+      <c r="I396" s="21"/>
     </row>
     <row r="397">
-      <c r="I397" s="20"/>
+      <c r="I397" s="21"/>
     </row>
     <row r="398">
-      <c r="I398" s="20"/>
+      <c r="I398" s="21"/>
     </row>
     <row r="399">
-      <c r="I399" s="20"/>
+      <c r="I399" s="21"/>
     </row>
     <row r="400">
-      <c r="I400" s="20"/>
+      <c r="I400" s="21"/>
     </row>
     <row r="401">
-      <c r="I401" s="20"/>
+      <c r="I401" s="21"/>
     </row>
     <row r="402">
-      <c r="I402" s="20"/>
+      <c r="I402" s="21"/>
     </row>
     <row r="403">
-      <c r="I403" s="20"/>
+      <c r="I403" s="21"/>
     </row>
     <row r="404">
-      <c r="I404" s="20"/>
+      <c r="I404" s="21"/>
     </row>
     <row r="405">
-      <c r="I405" s="20"/>
+      <c r="I405" s="21"/>
     </row>
     <row r="406">
-      <c r="I406" s="20"/>
+      <c r="I406" s="21"/>
     </row>
     <row r="407">
-      <c r="I407" s="20"/>
+      <c r="I407" s="21"/>
     </row>
     <row r="408">
-      <c r="I408" s="20"/>
+      <c r="I408" s="21"/>
     </row>
     <row r="409">
-      <c r="I409" s="20"/>
+      <c r="I409" s="21"/>
     </row>
     <row r="410">
-      <c r="I410" s="20"/>
+      <c r="I410" s="21"/>
     </row>
     <row r="411">
-      <c r="I411" s="20"/>
+      <c r="I411" s="21"/>
     </row>
     <row r="412">
-      <c r="I412" s="20"/>
+      <c r="I412" s="21"/>
     </row>
     <row r="413">
-      <c r="I413" s="20"/>
+      <c r="I413" s="21"/>
     </row>
     <row r="414">
-      <c r="I414" s="20"/>
+      <c r="I414" s="21"/>
     </row>
     <row r="415">
-      <c r="I415" s="20"/>
+      <c r="I415" s="21"/>
     </row>
     <row r="416">
-      <c r="I416" s="20"/>
+      <c r="I416" s="21"/>
     </row>
     <row r="417">
-      <c r="I417" s="20"/>
+      <c r="I417" s="21"/>
     </row>
     <row r="418">
-      <c r="I418" s="20"/>
+      <c r="I418" s="21"/>
     </row>
     <row r="419">
-      <c r="I419" s="20"/>
+      <c r="I419" s="21"/>
     </row>
     <row r="420">
-      <c r="I420" s="20"/>
+      <c r="I420" s="21"/>
     </row>
     <row r="421">
-      <c r="I421" s="20"/>
+      <c r="I421" s="21"/>
     </row>
     <row r="422">
-      <c r="I422" s="20"/>
+      <c r="I422" s="21"/>
     </row>
     <row r="423">
-      <c r="I423" s="20"/>
+      <c r="I423" s="21"/>
     </row>
     <row r="424">
-      <c r="I424" s="20"/>
+      <c r="I424" s="21"/>
     </row>
     <row r="425">
-      <c r="I425" s="20"/>
+      <c r="I425" s="21"/>
     </row>
     <row r="426">
-      <c r="I426" s="20"/>
+      <c r="I426" s="21"/>
     </row>
     <row r="427">
-      <c r="I427" s="20"/>
+      <c r="I427" s="21"/>
     </row>
     <row r="428">
-      <c r="I428" s="20"/>
+      <c r="I428" s="21"/>
     </row>
     <row r="429">
-      <c r="I429" s="20"/>
+      <c r="I429" s="21"/>
     </row>
     <row r="430">
-      <c r="I430" s="20"/>
+      <c r="I430" s="21"/>
     </row>
     <row r="431">
-      <c r="I431" s="20"/>
+      <c r="I431" s="21"/>
     </row>
     <row r="432">
-      <c r="I432" s="20"/>
+      <c r="I432" s="21"/>
     </row>
     <row r="433">
-      <c r="I433" s="20"/>
+      <c r="I433" s="21"/>
     </row>
     <row r="434">
-      <c r="I434" s="20"/>
+      <c r="I434" s="21"/>
     </row>
     <row r="435">
-      <c r="I435" s="20"/>
+      <c r="I435" s="21"/>
     </row>
     <row r="436">
-      <c r="I436" s="20"/>
+      <c r="I436" s="21"/>
     </row>
     <row r="437">
-      <c r="I437" s="20"/>
+      <c r="I437" s="21"/>
     </row>
     <row r="438">
-      <c r="I438" s="20"/>
+      <c r="I438" s="21"/>
     </row>
     <row r="439">
-      <c r="I439" s="20"/>
+      <c r="I439" s="21"/>
     </row>
     <row r="440">
-      <c r="I440" s="20"/>
+      <c r="I440" s="21"/>
     </row>
     <row r="441">
-      <c r="I441" s="20"/>
+      <c r="I441" s="21"/>
     </row>
     <row r="442">
-      <c r="I442" s="20"/>
+      <c r="I442" s="21"/>
     </row>
     <row r="443">
-      <c r="I443" s="20"/>
+      <c r="I443" s="21"/>
     </row>
     <row r="444">
-      <c r="I444" s="20"/>
+      <c r="I444" s="21"/>
     </row>
     <row r="445">
-      <c r="I445" s="20"/>
+      <c r="I445" s="21"/>
     </row>
     <row r="446">
-      <c r="I446" s="20"/>
+      <c r="I446" s="21"/>
     </row>
     <row r="447">
-      <c r="I447" s="20"/>
+      <c r="I447" s="21"/>
     </row>
     <row r="448">
-      <c r="I448" s="20"/>
+      <c r="I448" s="21"/>
     </row>
     <row r="449">
-      <c r="I449" s="20"/>
+      <c r="I449" s="21"/>
     </row>
     <row r="450">
-      <c r="I450" s="20"/>
+      <c r="I450" s="21"/>
     </row>
     <row r="451">
-      <c r="I451" s="20"/>
+      <c r="I451" s="21"/>
     </row>
     <row r="452">
-      <c r="I452" s="20"/>
+      <c r="I452" s="21"/>
     </row>
     <row r="453">
-      <c r="I453" s="20"/>
+      <c r="I453" s="21"/>
     </row>
     <row r="454">
-      <c r="I454" s="20"/>
+      <c r="I454" s="21"/>
     </row>
     <row r="455">
-      <c r="I455" s="20"/>
+      <c r="I455" s="21"/>
     </row>
     <row r="456">
-      <c r="I456" s="20"/>
+      <c r="I456" s="21"/>
     </row>
     <row r="457">
-      <c r="I457" s="20"/>
+      <c r="I457" s="21"/>
     </row>
     <row r="458">
-      <c r="I458" s="20"/>
+      <c r="I458" s="21"/>
     </row>
     <row r="459">
-      <c r="I459" s="20"/>
+      <c r="I459" s="21"/>
     </row>
     <row r="460">
-      <c r="I460" s="20"/>
+      <c r="I460" s="21"/>
     </row>
     <row r="461">
-      <c r="I461" s="20"/>
+      <c r="I461" s="21"/>
     </row>
     <row r="462">
-      <c r="I462" s="20"/>
+      <c r="I462" s="21"/>
     </row>
     <row r="463">
-      <c r="I463" s="20"/>
+      <c r="I463" s="21"/>
     </row>
     <row r="464">
-      <c r="I464" s="20"/>
+      <c r="I464" s="21"/>
     </row>
     <row r="465">
-      <c r="I465" s="20"/>
+      <c r="I465" s="21"/>
     </row>
     <row r="466">
-      <c r="I466" s="20"/>
+      <c r="I466" s="21"/>
     </row>
     <row r="467">
-      <c r="I467" s="20"/>
+      <c r="I467" s="21"/>
     </row>
     <row r="468">
-      <c r="I468" s="20"/>
+      <c r="I468" s="21"/>
     </row>
     <row r="469">
-      <c r="I469" s="20"/>
+      <c r="I469" s="21"/>
     </row>
     <row r="470">
-      <c r="I470" s="20"/>
+      <c r="I470" s="21"/>
     </row>
     <row r="471">
-      <c r="I471" s="20"/>
+      <c r="I471" s="21"/>
     </row>
     <row r="472">
-      <c r="I472" s="20"/>
+      <c r="I472" s="21"/>
     </row>
     <row r="473">
-      <c r="I473" s="20"/>
+      <c r="I473" s="21"/>
     </row>
     <row r="474">
-      <c r="I474" s="20"/>
+      <c r="I474" s="21"/>
     </row>
     <row r="475">
-      <c r="I475" s="20"/>
+      <c r="I475" s="21"/>
     </row>
     <row r="476">
-      <c r="I476" s="20"/>
+      <c r="I476" s="21"/>
     </row>
     <row r="477">
-      <c r="I477" s="20"/>
+      <c r="I477" s="21"/>
     </row>
     <row r="478">
-      <c r="I478" s="20"/>
+      <c r="I478" s="21"/>
     </row>
     <row r="479">
-      <c r="I479" s="20"/>
+      <c r="I479" s="21"/>
     </row>
     <row r="480">
-      <c r="I480" s="20"/>
+      <c r="I480" s="21"/>
     </row>
     <row r="481">
-      <c r="I481" s="20"/>
+      <c r="I481" s="21"/>
     </row>
     <row r="482">
-      <c r="I482" s="20"/>
+      <c r="I482" s="21"/>
     </row>
     <row r="483">
-      <c r="I483" s="20"/>
+      <c r="I483" s="21"/>
     </row>
     <row r="484">
-      <c r="I484" s="20"/>
+      <c r="I484" s="21"/>
     </row>
     <row r="485">
-      <c r="I485" s="20"/>
+      <c r="I485" s="21"/>
     </row>
     <row r="486">
-      <c r="I486" s="20"/>
+      <c r="I486" s="21"/>
     </row>
     <row r="487">
-      <c r="I487" s="20"/>
+      <c r="I487" s="21"/>
     </row>
     <row r="488">
-      <c r="I488" s="20"/>
+      <c r="I488" s="21"/>
     </row>
     <row r="489">
-      <c r="I489" s="20"/>
+      <c r="I489" s="21"/>
     </row>
     <row r="490">
-      <c r="I490" s="20"/>
+      <c r="I490" s="21"/>
     </row>
     <row r="491">
-      <c r="I491" s="20"/>
+      <c r="I491" s="21"/>
     </row>
     <row r="492">
-      <c r="I492" s="20"/>
+      <c r="I492" s="21"/>
     </row>
     <row r="493">
-      <c r="I493" s="20"/>
+      <c r="I493" s="21"/>
     </row>
     <row r="494">
-      <c r="I494" s="20"/>
+      <c r="I494" s="21"/>
     </row>
     <row r="495">
-      <c r="I495" s="20"/>
+      <c r="I495" s="21"/>
     </row>
     <row r="496">
-      <c r="I496" s="20"/>
+      <c r="I496" s="21"/>
     </row>
     <row r="497">
-      <c r="I497" s="20"/>
+      <c r="I497" s="21"/>
     </row>
     <row r="498">
-      <c r="I498" s="20"/>
+      <c r="I498" s="21"/>
     </row>
     <row r="499">
-      <c r="I499" s="20"/>
+      <c r="I499" s="21"/>
     </row>
     <row r="500">
-      <c r="I500" s="20"/>
+      <c r="I500" s="21"/>
     </row>
     <row r="501">
-      <c r="I501" s="20"/>
+      <c r="I501" s="21"/>
     </row>
     <row r="502">
-      <c r="I502" s="20"/>
+      <c r="I502" s="21"/>
     </row>
     <row r="503">
-      <c r="I503" s="20"/>
+      <c r="I503" s="21"/>
     </row>
     <row r="504">
-      <c r="I504" s="20"/>
+      <c r="I504" s="21"/>
     </row>
     <row r="505">
-      <c r="I505" s="20"/>
+      <c r="I505" s="21"/>
     </row>
     <row r="506">
-      <c r="I506" s="20"/>
+      <c r="I506" s="21"/>
     </row>
     <row r="507">
-      <c r="I507" s="20"/>
+      <c r="I507" s="21"/>
     </row>
     <row r="508">
-      <c r="I508" s="20"/>
+      <c r="I508" s="21"/>
     </row>
     <row r="509">
-      <c r="I509" s="20"/>
+      <c r="I509" s="21"/>
     </row>
     <row r="510">
-      <c r="I510" s="20"/>
+      <c r="I510" s="21"/>
     </row>
     <row r="511">
-      <c r="I511" s="20"/>
+      <c r="I511" s="21"/>
     </row>
     <row r="512">
-      <c r="I512" s="20"/>
+      <c r="I512" s="21"/>
     </row>
     <row r="513">
-      <c r="I513" s="20"/>
+      <c r="I513" s="21"/>
     </row>
     <row r="514">
-      <c r="I514" s="20"/>
+      <c r="I514" s="21"/>
     </row>
     <row r="515">
-      <c r="I515" s="20"/>
+      <c r="I515" s="21"/>
     </row>
     <row r="516">
-      <c r="I516" s="20"/>
+      <c r="I516" s="21"/>
     </row>
     <row r="517">
-      <c r="I517" s="20"/>
+      <c r="I517" s="21"/>
     </row>
     <row r="518">
-      <c r="I518" s="20"/>
+      <c r="I518" s="21"/>
     </row>
     <row r="519">
-      <c r="I519" s="20"/>
+      <c r="I519" s="21"/>
     </row>
     <row r="520">
-      <c r="I520" s="20"/>
+      <c r="I520" s="21"/>
     </row>
     <row r="521">
-      <c r="I521" s="20"/>
+      <c r="I521" s="21"/>
     </row>
     <row r="522">
-      <c r="I522" s="20"/>
+      <c r="I522" s="21"/>
     </row>
     <row r="523">
-      <c r="I523" s="20"/>
+      <c r="I523" s="21"/>
     </row>
     <row r="524">
-      <c r="I524" s="20"/>
+      <c r="I524" s="21"/>
     </row>
     <row r="525">
-      <c r="I525" s="20"/>
+      <c r="I525" s="21"/>
     </row>
     <row r="526">
-      <c r="I526" s="20"/>
+      <c r="I526" s="21"/>
     </row>
     <row r="527">
-      <c r="I527" s="20"/>
+      <c r="I527" s="21"/>
     </row>
     <row r="528">
-      <c r="I528" s="20"/>
+      <c r="I528" s="21"/>
     </row>
     <row r="529">
-      <c r="I529" s="20"/>
+      <c r="I529" s="21"/>
     </row>
     <row r="530">
-      <c r="I530" s="20"/>
+      <c r="I530" s="21"/>
     </row>
     <row r="531">
-      <c r="I531" s="20"/>
+      <c r="I531" s="21"/>
     </row>
     <row r="532">
-      <c r="I532" s="20"/>
+      <c r="I532" s="21"/>
     </row>
     <row r="533">
-      <c r="I533" s="20"/>
+      <c r="I533" s="21"/>
     </row>
     <row r="534">
-      <c r="I534" s="20"/>
+      <c r="I534" s="21"/>
     </row>
     <row r="535">
-      <c r="I535" s="20"/>
+      <c r="I535" s="21"/>
     </row>
     <row r="536">
-      <c r="I536" s="20"/>
+      <c r="I536" s="21"/>
     </row>
     <row r="537">
-      <c r="I537" s="20"/>
+      <c r="I537" s="21"/>
     </row>
     <row r="538">
-      <c r="I538" s="20"/>
+      <c r="I538" s="21"/>
     </row>
     <row r="539">
-      <c r="I539" s="20"/>
+      <c r="I539" s="21"/>
     </row>
     <row r="540">
-      <c r="I540" s="20"/>
+      <c r="I540" s="21"/>
     </row>
     <row r="541">
-      <c r="I541" s="20"/>
+      <c r="I541" s="21"/>
     </row>
     <row r="542">
-      <c r="I542" s="20"/>
+      <c r="I542" s="21"/>
     </row>
     <row r="543">
-      <c r="I543" s="20"/>
+      <c r="I543" s="21"/>
     </row>
     <row r="544">
-      <c r="I544" s="20"/>
+      <c r="I544" s="21"/>
     </row>
     <row r="545">
-      <c r="I545" s="20"/>
+      <c r="I545" s="21"/>
     </row>
     <row r="546">
-      <c r="I546" s="20"/>
+      <c r="I546" s="21"/>
     </row>
     <row r="547">
-      <c r="I547" s="20"/>
+      <c r="I547" s="21"/>
     </row>
     <row r="548">
-      <c r="I548" s="20"/>
+      <c r="I548" s="21"/>
     </row>
     <row r="549">
-      <c r="I549" s="20"/>
+      <c r="I549" s="21"/>
     </row>
     <row r="550">
-      <c r="I550" s="20"/>
+      <c r="I550" s="21"/>
     </row>
     <row r="551">
-      <c r="I551" s="20"/>
+      <c r="I551" s="21"/>
     </row>
     <row r="552">
-      <c r="I552" s="20"/>
+      <c r="I552" s="21"/>
     </row>
     <row r="553">
-      <c r="I553" s="20"/>
+      <c r="I553" s="21"/>
     </row>
     <row r="554">
-      <c r="I554" s="20"/>
+      <c r="I554" s="21"/>
     </row>
     <row r="555">
-      <c r="I555" s="20"/>
+      <c r="I555" s="21"/>
     </row>
     <row r="556">
-      <c r="I556" s="20"/>
+      <c r="I556" s="21"/>
     </row>
     <row r="557">
-      <c r="I557" s="20"/>
+      <c r="I557" s="21"/>
     </row>
     <row r="558">
-      <c r="I558" s="20"/>
+      <c r="I558" s="21"/>
     </row>
     <row r="559">
-      <c r="I559" s="20"/>
+      <c r="I559" s="21"/>
     </row>
     <row r="560">
-      <c r="I560" s="20"/>
+      <c r="I560" s="21"/>
     </row>
     <row r="561">
-      <c r="I561" s="20"/>
+      <c r="I561" s="21"/>
     </row>
     <row r="562">
-      <c r="I562" s="20"/>
+      <c r="I562" s="21"/>
     </row>
     <row r="563">
-      <c r="I563" s="20"/>
+      <c r="I563" s="21"/>
     </row>
     <row r="564">
-      <c r="I564" s="20"/>
+      <c r="I564" s="21"/>
     </row>
     <row r="565">
-      <c r="I565" s="20"/>
+      <c r="I565" s="21"/>
     </row>
     <row r="566">
-      <c r="I566" s="20"/>
+      <c r="I566" s="21"/>
     </row>
     <row r="567">
-      <c r="I567" s="20"/>
+      <c r="I567" s="21"/>
     </row>
     <row r="568">
-      <c r="I568" s="20"/>
+      <c r="I568" s="21"/>
     </row>
     <row r="569">
-      <c r="I569" s="20"/>
+      <c r="I569" s="21"/>
     </row>
     <row r="570">
-      <c r="I570" s="20"/>
+      <c r="I570" s="21"/>
     </row>
     <row r="571">
-      <c r="I571" s="20"/>
+      <c r="I571" s="21"/>
     </row>
     <row r="572">
-      <c r="I572" s="20"/>
+      <c r="I572" s="21"/>
     </row>
     <row r="573">
-      <c r="I573" s="20"/>
+      <c r="I573" s="21"/>
     </row>
     <row r="574">
-      <c r="I574" s="20"/>
+      <c r="I574" s="21"/>
     </row>
     <row r="575">
-      <c r="I575" s="20"/>
+      <c r="I575" s="21"/>
     </row>
     <row r="576">
-      <c r="I576" s="20"/>
+      <c r="I576" s="21"/>
     </row>
     <row r="577">
-      <c r="I577" s="20"/>
+      <c r="I577" s="21"/>
     </row>
     <row r="578">
-      <c r="I578" s="20"/>
+      <c r="I578" s="21"/>
     </row>
     <row r="579">
-      <c r="I579" s="20"/>
+      <c r="I579" s="21"/>
     </row>
     <row r="580">
-      <c r="I580" s="20"/>
+      <c r="I580" s="21"/>
     </row>
     <row r="581">
-      <c r="I581" s="20"/>
+      <c r="I581" s="21"/>
     </row>
     <row r="582">
-      <c r="I582" s="20"/>
+      <c r="I582" s="21"/>
     </row>
     <row r="583">
-      <c r="I583" s="20"/>
+      <c r="I583" s="21"/>
     </row>
     <row r="584">
-      <c r="I584" s="20"/>
+      <c r="I584" s="21"/>
     </row>
     <row r="585">
-      <c r="I585" s="20"/>
+      <c r="I585" s="21"/>
     </row>
     <row r="586">
-      <c r="I586" s="20"/>
+      <c r="I586" s="21"/>
     </row>
     <row r="587">
-      <c r="I587" s="20"/>
+      <c r="I587" s="21"/>
     </row>
     <row r="588">
-      <c r="I588" s="20"/>
+      <c r="I588" s="21"/>
     </row>
     <row r="589">
-      <c r="I589" s="20"/>
+      <c r="I589" s="21"/>
     </row>
     <row r="590">
-      <c r="I590" s="20"/>
+      <c r="I590" s="21"/>
     </row>
     <row r="591">
-      <c r="I591" s="20"/>
+      <c r="I591" s="21"/>
     </row>
     <row r="592">
-      <c r="I592" s="20"/>
+      <c r="I592" s="21"/>
     </row>
     <row r="593">
-      <c r="I593" s="20"/>
+      <c r="I593" s="21"/>
     </row>
     <row r="594">
-      <c r="I594" s="20"/>
+      <c r="I594" s="21"/>
     </row>
     <row r="595">
-      <c r="I595" s="20"/>
+      <c r="I595" s="21"/>
     </row>
     <row r="596">
-      <c r="I596" s="20"/>
+      <c r="I596" s="21"/>
     </row>
     <row r="597">
-      <c r="I597" s="20"/>
+      <c r="I597" s="21"/>
     </row>
     <row r="598">
-      <c r="I598" s="20"/>
+      <c r="I598" s="21"/>
     </row>
     <row r="599">
-      <c r="I599" s="20"/>
+      <c r="I599" s="21"/>
     </row>
     <row r="600">
-      <c r="I600" s="20"/>
+      <c r="I600" s="21"/>
     </row>
     <row r="601">
-      <c r="I601" s="20"/>
+      <c r="I601" s="21"/>
     </row>
     <row r="602">
-      <c r="I602" s="20"/>
+      <c r="I602" s="21"/>
     </row>
     <row r="603">
-      <c r="I603" s="20"/>
+      <c r="I603" s="21"/>
     </row>
     <row r="604">
-      <c r="I604" s="20"/>
+      <c r="I604" s="21"/>
     </row>
     <row r="605">
-      <c r="I605" s="20"/>
+      <c r="I605" s="21"/>
     </row>
     <row r="606">
-      <c r="I606" s="20"/>
+      <c r="I606" s="21"/>
     </row>
     <row r="607">
-      <c r="I607" s="20"/>
+      <c r="I607" s="21"/>
     </row>
     <row r="608">
-      <c r="I608" s="20"/>
+      <c r="I608" s="21"/>
     </row>
     <row r="609">
-      <c r="I609" s="20"/>
+      <c r="I609" s="21"/>
     </row>
     <row r="610">
-      <c r="I610" s="20"/>
+      <c r="I610" s="21"/>
     </row>
     <row r="611">
-      <c r="I611" s="20"/>
+      <c r="I611" s="21"/>
     </row>
     <row r="612">
-      <c r="I612" s="20"/>
+      <c r="I612" s="21"/>
     </row>
     <row r="613">
-      <c r="I613" s="20"/>
+      <c r="I613" s="21"/>
     </row>
     <row r="614">
-      <c r="I614" s="20"/>
+      <c r="I614" s="21"/>
     </row>
     <row r="615">
-      <c r="I615" s="20"/>
+      <c r="I615" s="21"/>
     </row>
     <row r="616">
-      <c r="I616" s="20"/>
+      <c r="I616" s="21"/>
     </row>
     <row r="617">
-      <c r="I617" s="20"/>
+      <c r="I617" s="21"/>
     </row>
     <row r="618">
-      <c r="I618" s="20"/>
+      <c r="I618" s="21"/>
     </row>
     <row r="619">
-      <c r="I619" s="20"/>
+      <c r="I619" s="21"/>
     </row>
     <row r="620">
-      <c r="I620" s="20"/>
+      <c r="I620" s="21"/>
     </row>
     <row r="621">
-      <c r="I621" s="20"/>
+      <c r="I621" s="21"/>
     </row>
     <row r="622">
-      <c r="I622" s="20"/>
+      <c r="I622" s="21"/>
     </row>
     <row r="623">
-      <c r="I623" s="20"/>
+      <c r="I623" s="21"/>
     </row>
     <row r="624">
-      <c r="I624" s="20"/>
+      <c r="I624" s="21"/>
     </row>
     <row r="625">
-      <c r="I625" s="20"/>
+      <c r="I625" s="21"/>
     </row>
     <row r="626">
-      <c r="I626" s="20"/>
+      <c r="I626" s="21"/>
     </row>
     <row r="627">
-      <c r="I627" s="20"/>
+      <c r="I627" s="21"/>
     </row>
     <row r="628">
-      <c r="I628" s="20"/>
+      <c r="I628" s="21"/>
     </row>
     <row r="629">
-      <c r="I629" s="20"/>
+      <c r="I629" s="21"/>
     </row>
     <row r="630">
-      <c r="I630" s="20"/>
+      <c r="I630" s="21"/>
     </row>
     <row r="631">
-      <c r="I631" s="20"/>
+      <c r="I631" s="21"/>
     </row>
     <row r="632">
-      <c r="I632" s="20"/>
+      <c r="I632" s="21"/>
     </row>
     <row r="633">
-      <c r="I633" s="20"/>
+      <c r="I633" s="21"/>
     </row>
     <row r="634">
-      <c r="I634" s="20"/>
+      <c r="I634" s="21"/>
     </row>
     <row r="635">
-      <c r="I635" s="20"/>
+      <c r="I635" s="21"/>
     </row>
     <row r="636">
-      <c r="I636" s="20"/>
+      <c r="I636" s="21"/>
     </row>
     <row r="637">
-      <c r="I637" s="20"/>
+      <c r="I637" s="21"/>
     </row>
     <row r="638">
-      <c r="I638" s="20"/>
+      <c r="I638" s="21"/>
     </row>
     <row r="639">
-      <c r="I639" s="20"/>
+      <c r="I639" s="21"/>
     </row>
     <row r="640">
-      <c r="I640" s="20"/>
+      <c r="I640" s="21"/>
     </row>
     <row r="641">
-      <c r="I641" s="20"/>
+      <c r="I641" s="21"/>
     </row>
     <row r="642">
-      <c r="I642" s="20"/>
+      <c r="I642" s="21"/>
     </row>
     <row r="643">
-      <c r="I643" s="20"/>
+      <c r="I643" s="21"/>
     </row>
     <row r="644">
-      <c r="I644" s="20"/>
+      <c r="I644" s="21"/>
     </row>
     <row r="645">
-      <c r="I645" s="20"/>
+      <c r="I645" s="21"/>
     </row>
     <row r="646">
-      <c r="I646" s="20"/>
+      <c r="I646" s="21"/>
     </row>
     <row r="647">
-      <c r="I647" s="20"/>
+      <c r="I647" s="21"/>
     </row>
     <row r="648">
-      <c r="I648" s="20"/>
+      <c r="I648" s="21"/>
     </row>
     <row r="649">
-      <c r="I649" s="20"/>
+      <c r="I649" s="21"/>
     </row>
     <row r="650">
-      <c r="I650" s="20"/>
+      <c r="I650" s="21"/>
     </row>
     <row r="651">
-      <c r="I651" s="20"/>
+      <c r="I651" s="21"/>
     </row>
     <row r="652">
-      <c r="I652" s="20"/>
+      <c r="I652" s="21"/>
     </row>
     <row r="653">
-      <c r="I653" s="20"/>
+      <c r="I653" s="21"/>
     </row>
     <row r="654">
-      <c r="I654" s="20"/>
+      <c r="I654" s="21"/>
     </row>
     <row r="655">
-      <c r="I655" s="20"/>
+      <c r="I655" s="21"/>
     </row>
     <row r="656">
-      <c r="I656" s="20"/>
+      <c r="I656" s="21"/>
     </row>
     <row r="657">
-      <c r="I657" s="20"/>
+      <c r="I657" s="21"/>
     </row>
     <row r="658">
-      <c r="I658" s="20"/>
+      <c r="I658" s="21"/>
     </row>
     <row r="659">
-      <c r="I659" s="20"/>
+      <c r="I659" s="21"/>
     </row>
     <row r="660">
-      <c r="I660" s="20"/>
+      <c r="I660" s="21"/>
     </row>
     <row r="661">
-      <c r="I661" s="20"/>
+      <c r="I661" s="21"/>
     </row>
     <row r="662">
-      <c r="I662" s="20"/>
+      <c r="I662" s="21"/>
     </row>
     <row r="663">
-      <c r="I663" s="20"/>
+      <c r="I663" s="21"/>
     </row>
     <row r="664">
-      <c r="I664" s="20"/>
+      <c r="I664" s="21"/>
     </row>
     <row r="665">
-      <c r="I665" s="20"/>
+      <c r="I665" s="21"/>
     </row>
     <row r="666">
-      <c r="I666" s="20"/>
+      <c r="I666" s="21"/>
     </row>
     <row r="667">
-      <c r="I667" s="20"/>
+      <c r="I667" s="21"/>
     </row>
     <row r="668">
-      <c r="I668" s="20"/>
+      <c r="I668" s="21"/>
     </row>
     <row r="669">
-      <c r="I669" s="20"/>
+      <c r="I669" s="21"/>
     </row>
     <row r="670">
-      <c r="I670" s="20"/>
+      <c r="I670" s="21"/>
     </row>
     <row r="671">
-      <c r="I671" s="20"/>
+      <c r="I671" s="21"/>
     </row>
     <row r="672">
-      <c r="I672" s="20"/>
+      <c r="I672" s="21"/>
     </row>
     <row r="673">
-      <c r="I673" s="20"/>
+      <c r="I673" s="21"/>
     </row>
     <row r="674">
-      <c r="I674" s="20"/>
+      <c r="I674" s="21"/>
     </row>
     <row r="675">
-      <c r="I675" s="20"/>
+      <c r="I675" s="21"/>
     </row>
     <row r="676">
-      <c r="I676" s="20"/>
+      <c r="I676" s="21"/>
     </row>
     <row r="677">
-      <c r="I677" s="20"/>
+      <c r="I677" s="21"/>
     </row>
     <row r="678">
-      <c r="I678" s="20"/>
+      <c r="I678" s="21"/>
     </row>
     <row r="679">
-      <c r="I679" s="20"/>
+      <c r="I679" s="21"/>
     </row>
     <row r="680">
-      <c r="I680" s="20"/>
+      <c r="I680" s="21"/>
     </row>
     <row r="681">
-      <c r="I681" s="20"/>
+      <c r="I681" s="21"/>
     </row>
     <row r="682">
-      <c r="I682" s="20"/>
+      <c r="I682" s="21"/>
     </row>
     <row r="683">
-      <c r="I683" s="20"/>
+      <c r="I683" s="21"/>
     </row>
     <row r="684">
-      <c r="I684" s="20"/>
+      <c r="I684" s="21"/>
     </row>
     <row r="685">
-      <c r="I685" s="20"/>
+      <c r="I685" s="21"/>
     </row>
     <row r="686">
-      <c r="I686" s="20"/>
+      <c r="I686" s="21"/>
     </row>
     <row r="687">
-      <c r="I687" s="20"/>
+      <c r="I687" s="21"/>
     </row>
     <row r="688">
-      <c r="I688" s="20"/>
+      <c r="I688" s="21"/>
     </row>
     <row r="689">
-      <c r="I689" s="20"/>
+      <c r="I689" s="21"/>
     </row>
     <row r="690">
-      <c r="I690" s="20"/>
+      <c r="I690" s="21"/>
     </row>
     <row r="691">
-      <c r="I691" s="20"/>
+      <c r="I691" s="21"/>
     </row>
     <row r="692">
-      <c r="I692" s="20"/>
+      <c r="I692" s="21"/>
     </row>
     <row r="693">
-      <c r="I693" s="20"/>
+      <c r="I693" s="21"/>
     </row>
     <row r="694">
-      <c r="I694" s="20"/>
+      <c r="I694" s="21"/>
     </row>
     <row r="695">
-      <c r="I695" s="20"/>
+      <c r="I695" s="21"/>
     </row>
     <row r="696">
-      <c r="I696" s="20"/>
+      <c r="I696" s="21"/>
     </row>
     <row r="697">
-      <c r="I697" s="20"/>
+      <c r="I697" s="21"/>
     </row>
     <row r="698">
-      <c r="I698" s="20"/>
+      <c r="I698" s="21"/>
     </row>
     <row r="699">
-      <c r="I699" s="20"/>
+      <c r="I699" s="21"/>
     </row>
     <row r="700">
-      <c r="I700" s="20"/>
+      <c r="I700" s="21"/>
     </row>
     <row r="701">
-      <c r="I701" s="20"/>
+      <c r="I701" s="21"/>
     </row>
     <row r="702">
-      <c r="I702" s="20"/>
+      <c r="I702" s="21"/>
     </row>
     <row r="703">
-      <c r="I703" s="20"/>
+      <c r="I703" s="21"/>
     </row>
     <row r="704">
-      <c r="I704" s="20"/>
+      <c r="I704" s="21"/>
     </row>
     <row r="705">
-      <c r="I705" s="20"/>
+      <c r="I705" s="21"/>
     </row>
     <row r="706">
-      <c r="I706" s="20"/>
+      <c r="I706" s="21"/>
     </row>
     <row r="707">
-      <c r="I707" s="20"/>
+      <c r="I707" s="21"/>
     </row>
     <row r="708">
-      <c r="I708" s="20"/>
+      <c r="I708" s="21"/>
     </row>
     <row r="709">
-      <c r="I709" s="20"/>
+      <c r="I709" s="21"/>
     </row>
     <row r="710">
-      <c r="I710" s="20"/>
+      <c r="I710" s="21"/>
     </row>
     <row r="711">
-      <c r="I711" s="20"/>
+      <c r="I711" s="21"/>
     </row>
     <row r="712">
-      <c r="I712" s="20"/>
+      <c r="I712" s="21"/>
     </row>
     <row r="713">
-      <c r="I713" s="20"/>
+      <c r="I713" s="21"/>
     </row>
     <row r="714">
-      <c r="I714" s="20"/>
+      <c r="I714" s="21"/>
     </row>
     <row r="715">
-      <c r="I715" s="20"/>
+      <c r="I715" s="21"/>
     </row>
     <row r="716">
-      <c r="I716" s="20"/>
+      <c r="I716" s="21"/>
     </row>
     <row r="717">
-      <c r="I717" s="20"/>
+      <c r="I717" s="21"/>
     </row>
     <row r="718">
-      <c r="I718" s="20"/>
+      <c r="I718" s="21"/>
     </row>
     <row r="719">
-      <c r="I719" s="20"/>
+      <c r="I719" s="21"/>
     </row>
     <row r="720">
-      <c r="I720" s="20"/>
+      <c r="I720" s="21"/>
     </row>
     <row r="721">
-      <c r="I721" s="20"/>
+      <c r="I721" s="21"/>
     </row>
     <row r="722">
-      <c r="I722" s="20"/>
+      <c r="I722" s="21"/>
     </row>
     <row r="723">
-      <c r="I723" s="20"/>
+      <c r="I723" s="21"/>
     </row>
     <row r="724">
-      <c r="I724" s="20"/>
+      <c r="I724" s="21"/>
     </row>
     <row r="725">
-      <c r="I725" s="20"/>
+      <c r="I725" s="21"/>
     </row>
     <row r="726">
-      <c r="I726" s="20"/>
+      <c r="I726" s="21"/>
     </row>
     <row r="727">
-      <c r="I727" s="20"/>
+      <c r="I727" s="21"/>
     </row>
     <row r="728">
-      <c r="I728" s="20"/>
+      <c r="I728" s="21"/>
     </row>
     <row r="729">
-      <c r="I729" s="20"/>
+      <c r="I729" s="21"/>
     </row>
     <row r="730">
-      <c r="I730" s="20"/>
+      <c r="I730" s="21"/>
     </row>
     <row r="731">
-      <c r="I731" s="20"/>
+      <c r="I731" s="21"/>
     </row>
     <row r="732">
-      <c r="I732" s="20"/>
+      <c r="I732" s="21"/>
     </row>
     <row r="733">
-      <c r="I733" s="20"/>
+      <c r="I733" s="21"/>
     </row>
     <row r="734">
-      <c r="I734" s="20"/>
+      <c r="I734" s="21"/>
     </row>
     <row r="735">
-      <c r="I735" s="20"/>
+      <c r="I735" s="21"/>
     </row>
     <row r="736">
-      <c r="I736" s="20"/>
+      <c r="I736" s="21"/>
     </row>
     <row r="737">
-      <c r="I737" s="20"/>
+      <c r="I737" s="21"/>
     </row>
     <row r="738">
-      <c r="I738" s="20"/>
+      <c r="I738" s="21"/>
     </row>
     <row r="739">
-      <c r="I739" s="20"/>
+      <c r="I739" s="21"/>
     </row>
     <row r="740">
-      <c r="I740" s="20"/>
+      <c r="I740" s="21"/>
     </row>
     <row r="741">
-      <c r="I741" s="20"/>
+      <c r="I741" s="21"/>
     </row>
     <row r="742">
-      <c r="I742" s="20"/>
+      <c r="I742" s="21"/>
     </row>
     <row r="743">
-      <c r="I743" s="20"/>
+      <c r="I743" s="21"/>
     </row>
     <row r="744">
-      <c r="I744" s="20"/>
+      <c r="I744" s="21"/>
     </row>
     <row r="745">
-      <c r="I745" s="20"/>
+      <c r="I745" s="21"/>
     </row>
     <row r="746">
-      <c r="I746" s="20"/>
+      <c r="I746" s="21"/>
     </row>
     <row r="747">
-      <c r="I747" s="20"/>
+      <c r="I747" s="21"/>
     </row>
     <row r="748">
-      <c r="I748" s="20"/>
+      <c r="I748" s="21"/>
     </row>
     <row r="749">
-      <c r="I749" s="20"/>
+      <c r="I749" s="21"/>
     </row>
     <row r="750">
-      <c r="I750" s="20"/>
+      <c r="I750" s="21"/>
     </row>
     <row r="751">
-      <c r="I751" s="20"/>
+      <c r="I751" s="21"/>
     </row>
     <row r="752">
-      <c r="I752" s="20"/>
+      <c r="I752" s="21"/>
     </row>
     <row r="753">
-      <c r="I753" s="20"/>
+      <c r="I753" s="21"/>
     </row>
     <row r="754">
-      <c r="I754" s="20"/>
+      <c r="I754" s="21"/>
     </row>
     <row r="755">
-      <c r="I755" s="20"/>
+      <c r="I755" s="21"/>
     </row>
     <row r="756">
-      <c r="I756" s="20"/>
+      <c r="I756" s="21"/>
     </row>
     <row r="757">
-      <c r="I757" s="20"/>
+      <c r="I757" s="21"/>
     </row>
     <row r="758">
-      <c r="I758" s="20"/>
+      <c r="I758" s="21"/>
     </row>
     <row r="759">
-      <c r="I759" s="20"/>
+      <c r="I759" s="21"/>
     </row>
     <row r="760">
-      <c r="I760" s="20"/>
+      <c r="I760" s="21"/>
     </row>
     <row r="761">
-      <c r="I761" s="20"/>
+      <c r="I761" s="21"/>
     </row>
     <row r="762">
-      <c r="I762" s="20"/>
+      <c r="I762" s="21"/>
     </row>
     <row r="763">
-      <c r="I763" s="20"/>
+      <c r="I763" s="21"/>
     </row>
     <row r="764">
-      <c r="I764" s="20"/>
+      <c r="I764" s="21"/>
     </row>
     <row r="765">
-      <c r="I765" s="20"/>
+      <c r="I765" s="21"/>
     </row>
     <row r="766">
-      <c r="I766" s="20"/>
+      <c r="I766" s="21"/>
     </row>
     <row r="767">
-      <c r="I767" s="20"/>
+      <c r="I767" s="21"/>
     </row>
     <row r="768">
-      <c r="I768" s="20"/>
+      <c r="I768" s="21"/>
     </row>
     <row r="769">
-      <c r="I769" s="20"/>
+      <c r="I769" s="21"/>
     </row>
     <row r="770">
-      <c r="I770" s="20"/>
+      <c r="I770" s="21"/>
     </row>
     <row r="771">
-      <c r="I771" s="20"/>
+      <c r="I771" s="21"/>
     </row>
     <row r="772">
-      <c r="I772" s="20"/>
+      <c r="I772" s="21"/>
     </row>
     <row r="773">
-      <c r="I773" s="20"/>
+      <c r="I773" s="21"/>
     </row>
     <row r="774">
-      <c r="I774" s="20"/>
+      <c r="I774" s="21"/>
     </row>
     <row r="775">
-      <c r="I775" s="20"/>
+      <c r="I775" s="21"/>
     </row>
     <row r="776">
-      <c r="I776" s="20"/>
+      <c r="I776" s="21"/>
     </row>
     <row r="777">
-      <c r="I777" s="20"/>
+      <c r="I777" s="21"/>
     </row>
     <row r="778">
-      <c r="I778" s="20"/>
+      <c r="I778" s="21"/>
     </row>
     <row r="779">
-      <c r="I779" s="20"/>
+      <c r="I779" s="21"/>
     </row>
     <row r="780">
-      <c r="I780" s="20"/>
+      <c r="I780" s="21"/>
     </row>
     <row r="781">
-      <c r="I781" s="20"/>
+      <c r="I781" s="21"/>
     </row>
     <row r="782">
-      <c r="I782" s="20"/>
+      <c r="I782" s="21"/>
     </row>
     <row r="783">
-      <c r="I783" s="20"/>
+      <c r="I783" s="21"/>
     </row>
     <row r="784">
-      <c r="I784" s="20"/>
+      <c r="I784" s="21"/>
     </row>
     <row r="785">
-      <c r="I785" s="20"/>
+      <c r="I785" s="21"/>
     </row>
     <row r="786">
-      <c r="I786" s="20"/>
+      <c r="I786" s="21"/>
     </row>
     <row r="787">
-      <c r="I787" s="20"/>
+      <c r="I787" s="21"/>
     </row>
     <row r="788">
-      <c r="I788" s="20"/>
+      <c r="I788" s="21"/>
     </row>
     <row r="789">
-      <c r="I789" s="20"/>
+      <c r="I789" s="21"/>
     </row>
     <row r="790">
-      <c r="I790" s="20"/>
+      <c r="I790" s="21"/>
     </row>
     <row r="791">
-      <c r="I791" s="20"/>
+      <c r="I791" s="21"/>
     </row>
     <row r="792">
-      <c r="I792" s="20"/>
+      <c r="I792" s="21"/>
     </row>
     <row r="793">
-      <c r="I793" s="20"/>
+      <c r="I793" s="21"/>
     </row>
     <row r="794">
-      <c r="I794" s="20"/>
+      <c r="I794" s="21"/>
     </row>
     <row r="795">
-      <c r="I795" s="20"/>
+      <c r="I795" s="21"/>
     </row>
     <row r="796">
-      <c r="I796" s="20"/>
+      <c r="I796" s="21"/>
     </row>
     <row r="797">
-      <c r="I797" s="20"/>
+      <c r="I797" s="21"/>
     </row>
     <row r="798">
-      <c r="I798" s="20"/>
+      <c r="I798" s="21"/>
     </row>
     <row r="799">
-      <c r="I799" s="20"/>
+      <c r="I799" s="21"/>
     </row>
     <row r="800">
-      <c r="I800" s="20"/>
+      <c r="I800" s="21"/>
     </row>
     <row r="801">
-      <c r="I801" s="20"/>
+      <c r="I801" s="21"/>
     </row>
     <row r="802">
-      <c r="I802" s="20"/>
+      <c r="I802" s="21"/>
     </row>
     <row r="803">
-      <c r="I803" s="20"/>
+      <c r="I803" s="21"/>
     </row>
     <row r="804">
-      <c r="I804" s="20"/>
+      <c r="I804" s="21"/>
     </row>
     <row r="805">
-      <c r="I805" s="20"/>
+      <c r="I805" s="21"/>
     </row>
     <row r="806">
-      <c r="I806" s="20"/>
+      <c r="I806" s="21"/>
     </row>
     <row r="807">
-      <c r="I807" s="20"/>
+      <c r="I807" s="21"/>
     </row>
     <row r="808">
-      <c r="I808" s="20"/>
+      <c r="I808" s="21"/>
     </row>
     <row r="809">
-      <c r="I809" s="20"/>
+      <c r="I809" s="21"/>
     </row>
     <row r="810">
-      <c r="I810" s="20"/>
+      <c r="I810" s="21"/>
     </row>
     <row r="811">
-      <c r="I811" s="20"/>
+      <c r="I811" s="21"/>
     </row>
     <row r="812">
-      <c r="I812" s="20"/>
+      <c r="I812" s="21"/>
     </row>
     <row r="813">
-      <c r="I813" s="20"/>
+      <c r="I813" s="21"/>
     </row>
     <row r="814">
-      <c r="I814" s="20"/>
+      <c r="I814" s="21"/>
     </row>
     <row r="815">
-      <c r="I815" s="20"/>
+      <c r="I815" s="21"/>
     </row>
     <row r="816">
-      <c r="I816" s="20"/>
+      <c r="I816" s="21"/>
     </row>
     <row r="817">
-      <c r="I817" s="20"/>
+      <c r="I817" s="21"/>
     </row>
     <row r="818">
-      <c r="I818" s="20"/>
+      <c r="I818" s="21"/>
     </row>
     <row r="819">
-      <c r="I819" s="20"/>
+      <c r="I819" s="21"/>
     </row>
     <row r="820">
-      <c r="I820" s="20"/>
+      <c r="I820" s="21"/>
     </row>
     <row r="821">
-      <c r="I821" s="20"/>
+      <c r="I821" s="21"/>
     </row>
     <row r="822">
-      <c r="I822" s="20"/>
+      <c r="I822" s="21"/>
     </row>
     <row r="823">
-      <c r="I823" s="20"/>
+      <c r="I823" s="21"/>
     </row>
     <row r="824">
-      <c r="I824" s="20"/>
+      <c r="I824" s="21"/>
     </row>
     <row r="825">
-      <c r="I825" s="20"/>
+      <c r="I825" s="21"/>
     </row>
     <row r="826">
-      <c r="I826" s="20"/>
+      <c r="I826" s="21"/>
     </row>
     <row r="827">
-      <c r="I827" s="20"/>
+      <c r="I827" s="21"/>
     </row>
     <row r="828">
-      <c r="I828" s="20"/>
+      <c r="I828" s="21"/>
     </row>
     <row r="829">
-      <c r="I829" s="20"/>
+      <c r="I829" s="21"/>
     </row>
     <row r="830">
-      <c r="I830" s="20"/>
+      <c r="I830" s="21"/>
     </row>
     <row r="831">
-      <c r="I831" s="20"/>
+      <c r="I831" s="21"/>
     </row>
     <row r="832">
-      <c r="I832" s="20"/>
+      <c r="I832" s="21"/>
     </row>
     <row r="833">
-      <c r="I833" s="20"/>
+      <c r="I833" s="21"/>
     </row>
     <row r="834">
-      <c r="I834" s="20"/>
+      <c r="I834" s="21"/>
     </row>
     <row r="835">
-      <c r="I835" s="20"/>
+      <c r="I835" s="21"/>
     </row>
     <row r="836">
-      <c r="I836" s="20"/>
+      <c r="I836" s="21"/>
     </row>
     <row r="837">
-      <c r="I837" s="20"/>
+      <c r="I837" s="21"/>
     </row>
     <row r="838">
-      <c r="I838" s="20"/>
+      <c r="I838" s="21"/>
     </row>
     <row r="839">
-      <c r="I839" s="20"/>
+      <c r="I839" s="21"/>
     </row>
     <row r="840">
-      <c r="I840" s="20"/>
+      <c r="I840" s="21"/>
     </row>
     <row r="841">
-      <c r="I841" s="20"/>
+      <c r="I841" s="21"/>
     </row>
     <row r="842">
-      <c r="I842" s="20"/>
+      <c r="I842" s="21"/>
     </row>
     <row r="843">
-      <c r="I843" s="20"/>
+      <c r="I843" s="21"/>
     </row>
     <row r="844">
-      <c r="I844" s="20"/>
+      <c r="I844" s="21"/>
     </row>
     <row r="845">
-      <c r="I845" s="20"/>
+      <c r="I845" s="21"/>
     </row>
     <row r="846">
-      <c r="I846" s="20"/>
+      <c r="I846" s="21"/>
     </row>
     <row r="847">
-      <c r="I847" s="20"/>
+      <c r="I847" s="21"/>
     </row>
     <row r="848">
-      <c r="I848" s="20"/>
+      <c r="I848" s="21"/>
     </row>
     <row r="849">
-      <c r="I849" s="20"/>
+      <c r="I849" s="21"/>
     </row>
     <row r="850">
-      <c r="I850" s="20"/>
+      <c r="I850" s="21"/>
     </row>
     <row r="851">
-      <c r="I851" s="20"/>
+      <c r="I851" s="21"/>
     </row>
     <row r="852">
-      <c r="I852" s="20"/>
+      <c r="I852" s="21"/>
     </row>
     <row r="853">
-      <c r="I853" s="20"/>
+      <c r="I853" s="21"/>
     </row>
     <row r="854">
-      <c r="I854" s="20"/>
+      <c r="I854" s="21"/>
     </row>
     <row r="855">
-      <c r="I855" s="20"/>
+      <c r="I855" s="21"/>
     </row>
     <row r="856">
-      <c r="I856" s="20"/>
+      <c r="I856" s="21"/>
     </row>
     <row r="857">
-      <c r="I857" s="20"/>
+      <c r="I857" s="21"/>
     </row>
     <row r="858">
-      <c r="I858" s="20"/>
+      <c r="I858" s="21"/>
     </row>
     <row r="859">
-      <c r="I859" s="20"/>
+      <c r="I859" s="21"/>
     </row>
     <row r="860">
-      <c r="I860" s="20"/>
+      <c r="I860" s="21"/>
     </row>
     <row r="861">
-      <c r="I861" s="20"/>
+      <c r="I861" s="21"/>
     </row>
     <row r="862">
-      <c r="I862" s="20"/>
+      <c r="I862" s="21"/>
     </row>
     <row r="863">
-      <c r="I863" s="20"/>
+      <c r="I863" s="21"/>
     </row>
     <row r="864">
-      <c r="I864" s="20"/>
+      <c r="I864" s="21"/>
     </row>
     <row r="865">
-      <c r="I865" s="20"/>
+      <c r="I865" s="21"/>
     </row>
     <row r="866">
-      <c r="I866" s="20"/>
+      <c r="I866" s="21"/>
     </row>
     <row r="867">
-      <c r="I867" s="20"/>
+      <c r="I867" s="21"/>
     </row>
     <row r="868">
-      <c r="I868" s="20"/>
+      <c r="I868" s="21"/>
     </row>
     <row r="869">
-      <c r="I869" s="20"/>
+      <c r="I869" s="21"/>
     </row>
     <row r="870">
-      <c r="I870" s="20"/>
+      <c r="I870" s="21"/>
     </row>
     <row r="871">
-      <c r="I871" s="20"/>
+      <c r="I871" s="21"/>
     </row>
     <row r="872">
-      <c r="I872" s="20"/>
+      <c r="I872" s="21"/>
     </row>
     <row r="873">
-      <c r="I873" s="20"/>
+      <c r="I873" s="21"/>
     </row>
     <row r="874">
-      <c r="I874" s="20"/>
+      <c r="I874" s="21"/>
     </row>
     <row r="875">
-      <c r="I875" s="20"/>
+      <c r="I875" s="21"/>
     </row>
     <row r="876">
-      <c r="I876" s="20"/>
+      <c r="I876" s="21"/>
     </row>
     <row r="877">
-      <c r="I877" s="20"/>
+      <c r="I877" s="21"/>
     </row>
     <row r="878">
-      <c r="I878" s="20"/>
+      <c r="I878" s="21"/>
     </row>
     <row r="879">
-      <c r="I879" s="20"/>
+      <c r="I879" s="21"/>
     </row>
     <row r="880">
-      <c r="I880" s="20"/>
+      <c r="I880" s="21"/>
     </row>
     <row r="881">
-      <c r="I881" s="20"/>
+      <c r="I881" s="21"/>
     </row>
     <row r="882">
-      <c r="I882" s="20"/>
+      <c r="I882" s="21"/>
     </row>
     <row r="883">
-      <c r="I883" s="20"/>
+      <c r="I883" s="21"/>
     </row>
     <row r="884">
-      <c r="I884" s="20"/>
+      <c r="I884" s="21"/>
     </row>
     <row r="885">
-      <c r="I885" s="20"/>
+      <c r="I885" s="21"/>
     </row>
     <row r="886">
-      <c r="I886" s="20"/>
+      <c r="I886" s="21"/>
     </row>
     <row r="887">
-      <c r="I887" s="20"/>
+      <c r="I887" s="21"/>
     </row>
     <row r="888">
-      <c r="I888" s="20"/>
+      <c r="I888" s="21"/>
     </row>
     <row r="889">
-      <c r="I889" s="20"/>
+      <c r="I889" s="21"/>
     </row>
     <row r="890">
-      <c r="I890" s="20"/>
+      <c r="I890" s="21"/>
     </row>
     <row r="891">
-      <c r="I891" s="20"/>
+      <c r="I891" s="21"/>
     </row>
     <row r="892">
-      <c r="I892" s="20"/>
+      <c r="I892" s="21"/>
     </row>
     <row r="893">
-      <c r="I893" s="20"/>
+      <c r="I893" s="21"/>
     </row>
     <row r="894">
-      <c r="I894" s="20"/>
+      <c r="I894" s="21"/>
     </row>
     <row r="895">
-      <c r="I895" s="20"/>
+      <c r="I895" s="21"/>
     </row>
     <row r="896">
-      <c r="I896" s="20"/>
+      <c r="I896" s="21"/>
     </row>
     <row r="897">
-      <c r="I897" s="20"/>
+      <c r="I897" s="21"/>
     </row>
     <row r="898">
-      <c r="I898" s="20"/>
+      <c r="I898" s="21"/>
     </row>
     <row r="899">
-      <c r="I899" s="20"/>
+      <c r="I899" s="21"/>
     </row>
     <row r="900">
-      <c r="I900" s="20"/>
+      <c r="I900" s="21"/>
     </row>
     <row r="901">
-      <c r="I901" s="20"/>
+      <c r="I901" s="21"/>
     </row>
     <row r="902">
-      <c r="I902" s="20"/>
+      <c r="I902" s="21"/>
     </row>
     <row r="903">
-      <c r="I903" s="20"/>
+      <c r="I903" s="21"/>
     </row>
     <row r="904">
-      <c r="I904" s="20"/>
+      <c r="I904" s="21"/>
     </row>
     <row r="905">
-      <c r="I905" s="20"/>
+      <c r="I905" s="21"/>
     </row>
     <row r="906">
-      <c r="I906" s="20"/>
+      <c r="I906" s="21"/>
     </row>
     <row r="907">
-      <c r="I907" s="20"/>
+      <c r="I907" s="21"/>
     </row>
     <row r="908">
-      <c r="I908" s="20"/>
+      <c r="I908" s="21"/>
     </row>
     <row r="909">
-      <c r="I909" s="20"/>
+      <c r="I909" s="21"/>
     </row>
     <row r="910">
-      <c r="I910" s="20"/>
+      <c r="I910" s="21"/>
     </row>
     <row r="911">
-      <c r="I911" s="20"/>
+      <c r="I911" s="21"/>
     </row>
     <row r="912">
-      <c r="I912" s="20"/>
+      <c r="I912" s="21"/>
     </row>
     <row r="913">
-      <c r="I913" s="20"/>
+      <c r="I913" s="21"/>
     </row>
     <row r="914">
-      <c r="I914" s="20"/>
+      <c r="I914" s="21"/>
     </row>
     <row r="915">
-      <c r="I915" s="20"/>
+      <c r="I915" s="21"/>
     </row>
     <row r="916">
-      <c r="I916" s="20"/>
+      <c r="I916" s="21"/>
     </row>
     <row r="917">
-      <c r="I917" s="20"/>
+      <c r="I917" s="21"/>
     </row>
     <row r="918">
-      <c r="I918" s="20"/>
+      <c r="I918" s="21"/>
     </row>
     <row r="919">
-      <c r="I919" s="20"/>
+      <c r="I919" s="21"/>
     </row>
     <row r="920">
-      <c r="I920" s="20"/>
+      <c r="I920" s="21"/>
     </row>
     <row r="921">
-      <c r="I921" s="20"/>
+      <c r="I921" s="21"/>
     </row>
     <row r="922">
-      <c r="I922" s="20"/>
+      <c r="I922" s="21"/>
     </row>
     <row r="923">
-      <c r="I923" s="20"/>
+      <c r="I923" s="21"/>
     </row>
     <row r="924">
-      <c r="I924" s="20"/>
+      <c r="I924" s="21"/>
     </row>
     <row r="925">
-      <c r="I925" s="20"/>
+      <c r="I925" s="21"/>
     </row>
     <row r="926">
-      <c r="I926" s="20"/>
+      <c r="I926" s="21"/>
     </row>
     <row r="927">
-      <c r="I927" s="20"/>
+      <c r="I927" s="21"/>
     </row>
     <row r="928">
-      <c r="I928" s="20"/>
+      <c r="I928" s="21"/>
     </row>
     <row r="929">
-      <c r="I929" s="20"/>
+      <c r="I929" s="21"/>
     </row>
     <row r="930">
-      <c r="I930" s="20"/>
+      <c r="I930" s="21"/>
     </row>
     <row r="931">
-      <c r="I931" s="20"/>
+      <c r="I931" s="21"/>
     </row>
     <row r="932">
-      <c r="I932" s="20"/>
+      <c r="I932" s="21"/>
     </row>
     <row r="933">
-      <c r="I933" s="20"/>
+      <c r="I933" s="21"/>
     </row>
     <row r="934">
-      <c r="I934" s="20"/>
+      <c r="I934" s="21"/>
     </row>
     <row r="935">
-      <c r="I935" s="20"/>
+      <c r="I935" s="21"/>
     </row>
     <row r="936">
-      <c r="I936" s="20"/>
+      <c r="I936" s="21"/>
     </row>
     <row r="937">
-      <c r="I937" s="20"/>
+      <c r="I937" s="21"/>
     </row>
     <row r="938">
-      <c r="I938" s="20"/>
+      <c r="I938" s="21"/>
     </row>
     <row r="939">
-      <c r="I939" s="20"/>
+      <c r="I939" s="21"/>
     </row>
     <row r="940">
-      <c r="I940" s="20"/>
+      <c r="I940" s="21"/>
     </row>
     <row r="941">
-      <c r="I941" s="20"/>
+      <c r="I941" s="21"/>
     </row>
     <row r="942">
-      <c r="I942" s="20"/>
+      <c r="I942" s="21"/>
     </row>
     <row r="943">
-      <c r="I943" s="20"/>
+      <c r="I943" s="21"/>
     </row>
     <row r="944">
-      <c r="I944" s="20"/>
+      <c r="I944" s="21"/>
     </row>
     <row r="945">
-      <c r="I945" s="20"/>
+      <c r="I945" s="21"/>
     </row>
     <row r="946">
-      <c r="I946" s="20"/>
+      <c r="I946" s="21"/>
     </row>
     <row r="947">
-      <c r="I947" s="20"/>
+      <c r="I947" s="21"/>
     </row>
     <row r="948">
-      <c r="I948" s="20"/>
+      <c r="I948" s="21"/>
     </row>
     <row r="949">
-      <c r="I949" s="20"/>
+      <c r="I949" s="21"/>
     </row>
     <row r="950">
-      <c r="I950" s="20"/>
+      <c r="I950" s="21"/>
     </row>
     <row r="951">
-      <c r="I951" s="20"/>
+      <c r="I951" s="21"/>
     </row>
     <row r="952">
-      <c r="I952" s="20"/>
+      <c r="I952" s="21"/>
     </row>
     <row r="953">
-      <c r="I953" s="20"/>
+      <c r="I953" s="21"/>
     </row>
     <row r="954">
-      <c r="I954" s="20"/>
+      <c r="I954" s="21"/>
     </row>
     <row r="955">
-      <c r="I955" s="20"/>
+      <c r="I955" s="21"/>
     </row>
     <row r="956">
-      <c r="I956" s="20"/>
+      <c r="I956" s="21"/>
     </row>
     <row r="957">
-      <c r="I957" s="20"/>
+      <c r="I957" s="21"/>
     </row>
     <row r="958">
-      <c r="I958" s="20"/>
+      <c r="I958" s="21"/>
     </row>
     <row r="959">
-      <c r="I959" s="20"/>
+      <c r="I959" s="21"/>
     </row>
     <row r="960">
-      <c r="I960" s="20"/>
+      <c r="I960" s="21"/>
     </row>
     <row r="961">
-      <c r="I961" s="20"/>
+      <c r="I961" s="21"/>
     </row>
     <row r="962">
-      <c r="I962" s="20"/>
+      <c r="I962" s="21"/>
     </row>
     <row r="963">
-      <c r="I963" s="20"/>
+      <c r="I963" s="21"/>
     </row>
     <row r="964">
-      <c r="I964" s="20"/>
+      <c r="I964" s="21"/>
     </row>
     <row r="965">
-      <c r="I965" s="20"/>
+      <c r="I965" s="21"/>
     </row>
     <row r="966">
-      <c r="I966" s="20"/>
+      <c r="I966" s="21"/>
     </row>
     <row r="967">
-      <c r="I967" s="20"/>
+      <c r="I967" s="21"/>
     </row>
     <row r="968">
-      <c r="I968" s="20"/>
+      <c r="I968" s="21"/>
     </row>
     <row r="969">
-      <c r="I969" s="20"/>
+      <c r="I969" s="21"/>
     </row>
     <row r="970">
-      <c r="I970" s="20"/>
+      <c r="I970" s="21"/>
     </row>
     <row r="971">
-      <c r="I971" s="20"/>
+      <c r="I971" s="21"/>
     </row>
     <row r="972">
-      <c r="I972" s="20"/>
+      <c r="I972" s="21"/>
     </row>
     <row r="973">
-      <c r="I973" s="20"/>
+      <c r="I973" s="21"/>
     </row>
     <row r="974">
-      <c r="I974" s="20"/>
+      <c r="I974" s="21"/>
     </row>
     <row r="975">
-      <c r="I975" s="20"/>
+      <c r="I975" s="21"/>
     </row>
     <row r="976">
-      <c r="I976" s="20"/>
+      <c r="I976" s="21"/>
     </row>
     <row r="977">
-      <c r="I977" s="20"/>
+      <c r="I977" s="21"/>
     </row>
     <row r="978">
-      <c r="I978" s="20"/>
+      <c r="I978" s="21"/>
     </row>
     <row r="979">
-      <c r="I979" s="20"/>
+      <c r="I979" s="21"/>
     </row>
     <row r="980">
-      <c r="I980" s="20"/>
+      <c r="I980" s="21"/>
     </row>
     <row r="981">
-      <c r="I981" s="20"/>
+      <c r="I981" s="21"/>
     </row>
     <row r="982">
-      <c r="I982" s="20"/>
+      <c r="I982" s="21"/>
     </row>
     <row r="983">
-      <c r="I983" s="20"/>
+      <c r="I983" s="21"/>
     </row>
     <row r="984">
-      <c r="I984" s="20"/>
+      <c r="I984" s="21"/>
     </row>
     <row r="985">
-      <c r="I985" s="20"/>
+      <c r="I985" s="21"/>
     </row>
     <row r="986">
-      <c r="I986" s="20"/>
+      <c r="I986" s="21"/>
     </row>
     <row r="987">
-      <c r="I987" s="20"/>
+      <c r="I987" s="21"/>
     </row>
     <row r="988">
-      <c r="I988" s="20"/>
+      <c r="I988" s="21"/>
     </row>
     <row r="989">
-      <c r="I989" s="20"/>
+      <c r="I989" s="21"/>
     </row>
     <row r="990">
-      <c r="I990" s="20"/>
+      <c r="I990" s="21"/>
     </row>
     <row r="991">
-      <c r="I991" s="20"/>
+      <c r="I991" s="21"/>
     </row>
     <row r="992">
-      <c r="I992" s="20"/>
+      <c r="I992" s="21"/>
     </row>
     <row r="993">
-      <c r="I993" s="20"/>
+      <c r="I993" s="21"/>
     </row>
     <row r="994">
-      <c r="I994" s="20"/>
+      <c r="I994" s="21"/>
     </row>
     <row r="995">
-      <c r="I995" s="20"/>
+      <c r="I995" s="21"/>
     </row>
     <row r="996">
-      <c r="I996" s="20"/>
+      <c r="I996" s="21"/>
     </row>
     <row r="997">
-      <c r="I997" s="20"/>
+      <c r="I997" s="21"/>
     </row>
     <row r="998">
-      <c r="I998" s="20"/>
+      <c r="I998" s="21"/>
     </row>
     <row r="999">
-      <c r="I999" s="20"/>
+      <c r="I999" s="21"/>
+    </row>
+    <row r="1000">
+      <c r="I1000" s="21"/>
+    </row>
+    <row r="1001">
+      <c r="I1001" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>